<commit_message>
efficacy prototype hand-fit and kinda works
</commit_message>
<xml_diff>
--- a/data/typhoid_vaccine_study_data.xlsx
+++ b/data/typhoid_vaccine_study_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/famulare/git/famulare/typhoid-immune-dynamics/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F11104D-8755-EB4C-B109-F9242FA8F02B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFFE34F2-5E76-4E4A-9E65-8E8FBE73A170}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15020" yWindow="840" windowWidth="19540" windowHeight="17440" xr2:uid="{3C28E045-1CB7-C04C-9830-A174AB0F25A4}"/>
+    <workbookView xWindow="960" yWindow="840" windowWidth="33600" windowHeight="17440" xr2:uid="{3C28E045-1CB7-C04C-9830-A174AB0F25A4}"/>
   </bookViews>
   <sheets>
     <sheet name="efficacy" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2863" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2897" uniqueCount="311">
   <si>
     <t>study</t>
   </si>
@@ -971,6 +971,9 @@
   </si>
   <si>
     <t>17</t>
+  </si>
+  <si>
+    <t>fever&gt;=38</t>
   </si>
 </sst>
 </file>
@@ -1032,7 +1035,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1043,7 +1046,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1379,11 +1381,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E976F573-8D26-E847-8FB6-13AA5974A482}">
-  <dimension ref="A1:AH66"/>
+  <dimension ref="A1:AH68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="V66" sqref="V66"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AD44" sqref="AD44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4032,7 +4034,7 @@
       <c r="A30" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="8" t="s">
         <v>221</v>
       </c>
       <c r="C30">
@@ -4466,7 +4468,7 @@
         <v>22</v>
       </c>
       <c r="AD34" s="6">
-        <f t="shared" ref="AD34:AD37" si="0">(1-(Z34/X34)/(AA34/Y34))*100</f>
+        <f>(1-(Z34/X34)/(AA34/Y34))*100</f>
         <v>16.216216216216218</v>
       </c>
       <c r="AG34" s="3">
@@ -4553,7 +4555,7 @@
         <v>22</v>
       </c>
       <c r="AD35" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="AD35:AD39" si="0">(1-(Z35/X35)/(AA35/Y35))*100</f>
         <v>15.454545454545466</v>
       </c>
       <c r="AG35" s="3">
@@ -4589,7 +4591,7 @@
         <v>60</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>230</v>
+        <v>310</v>
       </c>
       <c r="L36" s="1" t="s">
         <v>21</v>
@@ -4628,20 +4630,20 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="X36" s="2">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="Y36" s="2">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="Z36" s="3">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="AA36" s="3">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AD36" s="6">
         <f t="shared" si="0"/>
-        <v>-16.599190283400823</v>
+        <v>70.42925278219397</v>
       </c>
       <c r="AG36" s="3">
         <v>95</v>
@@ -4676,7 +4678,7 @@
         <v>60</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>230</v>
+        <v>310</v>
       </c>
       <c r="L37" s="1" t="s">
         <v>21</v>
@@ -4715,20 +4717,20 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="X37" s="2">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="Y37" s="2">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="Z37" s="3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AA37" s="3">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AD37" s="6">
         <f t="shared" si="0"/>
-        <v>2.8340080971659853</v>
+        <v>42.689075630252091</v>
       </c>
       <c r="AG37" s="3">
         <v>95</v>
@@ -4745,7 +4747,7 @@
         <v>2017</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>13</v>
@@ -4769,7 +4771,7 @@
         <v>21</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>231</v>
+        <v>17</v>
       </c>
       <c r="N38" s="1" t="s">
         <v>299</v>
@@ -4787,7 +4789,7 @@
         <v>226</v>
       </c>
       <c r="S38" s="1" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="T38" s="1" t="s">
         <v>61</v>
@@ -4802,19 +4804,23 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="X38" s="2">
-        <v>31</v>
+        <v>13</v>
+      </c>
+      <c r="Y38" s="2">
+        <v>24</v>
+      </c>
+      <c r="Z38" s="3">
+        <v>12</v>
+      </c>
+      <c r="AA38" s="3">
+        <v>19</v>
       </c>
       <c r="AD38" s="6">
-        <v>0.4</v>
-      </c>
-      <c r="AE38" s="6">
-        <v>0.05</v>
-      </c>
-      <c r="AF38" s="6">
-        <v>22.7</v>
+        <f t="shared" si="0"/>
+        <v>-16.599190283400823</v>
       </c>
       <c r="AG38" s="3">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="39" spans="1:33" x14ac:dyDescent="0.2">
@@ -4828,7 +4834,7 @@
         <v>2017</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>240</v>
+        <v>222</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>13</v>
@@ -4852,7 +4858,7 @@
         <v>21</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>231</v>
+        <v>17</v>
       </c>
       <c r="N39" s="1" t="s">
         <v>299</v>
@@ -4870,7 +4876,7 @@
         <v>226</v>
       </c>
       <c r="S39" s="1" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="T39" s="1" t="s">
         <v>61</v>
@@ -4885,19 +4891,23 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="X39" s="2">
-        <v>37</v>
+        <v>13</v>
+      </c>
+      <c r="Y39" s="2">
+        <v>24</v>
+      </c>
+      <c r="Z39" s="3">
+        <v>10</v>
+      </c>
+      <c r="AA39" s="3">
+        <v>19</v>
       </c>
       <c r="AD39" s="6">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="AE39" s="6">
-        <v>0.05</v>
-      </c>
-      <c r="AF39" s="6">
-        <v>1.2</v>
+        <f t="shared" si="0"/>
+        <v>2.8340080971659853</v>
       </c>
       <c r="AG39" s="3">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="40" spans="1:33" x14ac:dyDescent="0.2">
@@ -4911,7 +4921,7 @@
         <v>2017</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>222</v>
+        <v>233</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>13</v>
@@ -4968,16 +4978,16 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="X40" s="2">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="AD40" s="6">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="AE40" s="6">
         <v>0.05</v>
       </c>
       <c r="AF40" s="6">
-        <v>5.6</v>
+        <v>22.7</v>
       </c>
       <c r="AG40" s="3">
         <v>100</v>
@@ -5012,13 +5022,13 @@
         <v>60</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="L41" s="1" t="s">
         <v>21</v>
       </c>
       <c r="M41" s="1" t="s">
-        <v>17</v>
+        <v>231</v>
       </c>
       <c r="N41" s="1" t="s">
         <v>299</v>
@@ -5027,7 +5037,7 @@
         <v>300</v>
       </c>
       <c r="P41" s="1" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="Q41" s="1" t="s">
         <v>145</v>
@@ -5036,7 +5046,7 @@
         <v>226</v>
       </c>
       <c r="S41" s="1" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="T41" s="1" t="s">
         <v>61</v>
@@ -5051,23 +5061,19 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="X41" s="2">
-        <v>13</v>
-      </c>
-      <c r="Y41" s="2">
-        <v>24</v>
-      </c>
-      <c r="Z41" s="3">
-        <v>11</v>
-      </c>
-      <c r="AA41" s="3">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="AD41" s="6">
-        <f t="shared" ref="AD41:AD42" si="1">(1-(Z41/X41)/(AA41/Y41))*100</f>
-        <v>15.384615384615385</v>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="AE41" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="AF41" s="6">
+        <v>1.2</v>
       </c>
       <c r="AG41" s="3">
-        <v>95</v>
+        <v>100</v>
       </c>
     </row>
     <row r="42" spans="1:33" x14ac:dyDescent="0.2">
@@ -5099,13 +5105,13 @@
         <v>60</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="L42" s="1" t="s">
         <v>21</v>
       </c>
       <c r="M42" s="1" t="s">
-        <v>17</v>
+        <v>231</v>
       </c>
       <c r="N42" s="1" t="s">
         <v>299</v>
@@ -5114,7 +5120,7 @@
         <v>300</v>
       </c>
       <c r="P42" s="1" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="Q42" s="1" t="s">
         <v>145</v>
@@ -5123,7 +5129,7 @@
         <v>226</v>
       </c>
       <c r="S42" s="1" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="T42" s="1" t="s">
         <v>61</v>
@@ -5138,23 +5144,19 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="X42" s="2">
-        <v>13</v>
-      </c>
-      <c r="Y42" s="2">
-        <v>24</v>
-      </c>
-      <c r="Z42" s="3">
-        <v>13</v>
-      </c>
-      <c r="AA42" s="3">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="AD42" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.1</v>
+      </c>
+      <c r="AE42" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="AF42" s="6">
+        <v>5.6</v>
       </c>
       <c r="AG42" s="3">
-        <v>95</v>
+        <v>100</v>
       </c>
     </row>
     <row r="43" spans="1:33" x14ac:dyDescent="0.2">
@@ -5186,7 +5188,7 @@
         <v>60</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="L43" s="1" t="s">
         <v>21</v>
@@ -5201,7 +5203,7 @@
         <v>300</v>
       </c>
       <c r="P43" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="Q43" s="1" t="s">
         <v>145</v>
@@ -5231,14 +5233,14 @@
         <v>24</v>
       </c>
       <c r="Z43" s="3">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="AA43" s="3">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="AD43" s="6">
-        <f>(1-(Z43/X43)/(AA43/Y43))*100</f>
-        <v>60.439560439560445</v>
+        <f t="shared" ref="AD43:AD44" si="1">(1-(Z43/X43)/(AA43/Y43))*100</f>
+        <v>15.384615384615385</v>
       </c>
       <c r="AG43" s="3">
         <v>95</v>
@@ -5273,7 +5275,7 @@
         <v>60</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="L44" s="1" t="s">
         <v>21</v>
@@ -5288,7 +5290,7 @@
         <v>300</v>
       </c>
       <c r="P44" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="Q44" s="1" t="s">
         <v>145</v>
@@ -5318,14 +5320,14 @@
         <v>24</v>
       </c>
       <c r="Z44" s="3">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="AA44" s="3">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="AD44" s="6">
-        <f>(1-(Z44/X44)/(AA44/Y44))*100</f>
-        <v>20.879120879120883</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="AG44" s="3">
         <v>95</v>
@@ -5333,13 +5335,13 @@
     </row>
     <row r="45" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>248</v>
+        <v>220</v>
       </c>
       <c r="B45" t="s">
-        <v>247</v>
+        <v>221</v>
       </c>
       <c r="C45">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>240</v>
@@ -5348,19 +5350,19 @@
         <v>13</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>238</v>
+        <v>223</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>304</v>
       </c>
       <c r="I45">
-        <v>0.75</v>
+        <v>18</v>
       </c>
       <c r="J45">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>11</v>
+        <v>235</v>
       </c>
       <c r="L45" s="1" t="s">
         <v>21</v>
@@ -5369,13 +5371,13 @@
         <v>17</v>
       </c>
       <c r="N45" s="1" t="s">
-        <v>279</v>
+        <v>299</v>
       </c>
       <c r="O45" s="1" t="s">
         <v>300</v>
       </c>
       <c r="P45" s="1" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="Q45" s="1" t="s">
         <v>145</v>
@@ -5384,40 +5386,35 @@
         <v>226</v>
       </c>
       <c r="S45" s="1" t="s">
-        <v>25</v>
+        <v>227</v>
       </c>
       <c r="T45" s="1" t="s">
-        <v>160</v>
+        <v>61</v>
       </c>
       <c r="U45" s="1" t="s">
-        <v>167</v>
+        <v>98</v>
       </c>
       <c r="V45">
         <v>1</v>
       </c>
       <c r="W45">
-        <v>12</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="X45" s="2">
-        <v>10005</v>
+        <v>13</v>
       </c>
       <c r="Y45" s="2">
-        <v>10014</v>
+        <v>24</v>
       </c>
       <c r="Z45" s="3">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="AA45" s="3">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="AD45" s="6">
-        <v>81.599999999999994</v>
-      </c>
-      <c r="AE45" s="6">
-        <v>58.8</v>
-      </c>
-      <c r="AF45" s="6">
-        <v>91.8</v>
+        <f>(1-(Z45/X45)/(AA45/Y45))*100</f>
+        <v>60.439560439560445</v>
       </c>
       <c r="AG45" s="3">
         <v>95</v>
@@ -5425,37 +5422,34 @@
     </row>
     <row r="46" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>236</v>
+        <v>220</v>
       </c>
       <c r="B46" t="s">
-        <v>237</v>
+        <v>221</v>
       </c>
       <c r="C46">
-        <v>2021</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>239</v>
+        <v>2017</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>240</v>
+        <v>222</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>238</v>
+        <v>223</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>304</v>
       </c>
       <c r="I46">
-        <v>0.75</v>
+        <v>18</v>
       </c>
       <c r="J46">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>11</v>
+        <v>235</v>
       </c>
       <c r="L46" s="1" t="s">
         <v>21</v>
@@ -5464,13 +5458,13 @@
         <v>17</v>
       </c>
       <c r="N46" s="1" t="s">
-        <v>279</v>
+        <v>299</v>
       </c>
       <c r="O46" s="1" t="s">
         <v>300</v>
       </c>
       <c r="P46" s="1" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="Q46" s="1" t="s">
         <v>145</v>
@@ -5479,46 +5473,35 @@
         <v>226</v>
       </c>
       <c r="S46" s="1" t="s">
-        <v>25</v>
+        <v>227</v>
       </c>
       <c r="T46" s="1" t="s">
-        <v>166</v>
+        <v>61</v>
       </c>
       <c r="U46" s="1" t="s">
-        <v>167</v>
+        <v>98</v>
       </c>
       <c r="V46">
         <v>1</v>
       </c>
       <c r="W46">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="X46" s="2">
+        <v>13</v>
+      </c>
+      <c r="Y46" s="2">
         <v>24</v>
       </c>
-      <c r="X46" s="2">
-        <v>10005</v>
-      </c>
-      <c r="Y46" s="2">
-        <v>10014</v>
-      </c>
       <c r="Z46" s="3">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="AA46" s="3">
-        <v>62</v>
-      </c>
-      <c r="AB46" s="3">
-        <v>18145</v>
-      </c>
-      <c r="AC46" s="3">
-        <v>18154</v>
+        <v>14</v>
       </c>
       <c r="AD46" s="6">
-        <v>79</v>
-      </c>
-      <c r="AE46" s="6">
-        <v>61.9</v>
-      </c>
-      <c r="AF46" s="6">
-        <v>88.5</v>
+        <f>(1-(Z46/X46)/(AA46/Y46))*100</f>
+        <v>20.879120879120883</v>
       </c>
       <c r="AG46" s="3">
         <v>95</v>
@@ -5526,16 +5509,13 @@
     </row>
     <row r="47" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>236</v>
+        <v>248</v>
       </c>
       <c r="B47" t="s">
-        <v>237</v>
+        <v>247</v>
       </c>
       <c r="C47">
-        <v>2021</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>239</v>
+        <v>2019</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>240</v>
@@ -5550,10 +5530,10 @@
         <v>304</v>
       </c>
       <c r="I47">
-        <v>2</v>
+        <v>0.75</v>
       </c>
       <c r="J47">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="K47" s="1" t="s">
         <v>11</v>
@@ -5568,13 +5548,13 @@
         <v>279</v>
       </c>
       <c r="O47" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="P47" s="1" t="s">
         <v>58</v>
       </c>
       <c r="Q47" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="R47" s="1" t="s">
         <v>226</v>
@@ -5583,39 +5563,37 @@
         <v>25</v>
       </c>
       <c r="T47" s="1" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="U47" s="1" t="s">
-        <v>307</v>
+        <v>167</v>
       </c>
       <c r="V47">
         <v>1</v>
       </c>
       <c r="W47">
-        <v>24</v>
+        <v>12</v>
+      </c>
+      <c r="X47" s="2">
+        <v>10005</v>
+      </c>
+      <c r="Y47" s="2">
+        <v>10014</v>
       </c>
       <c r="Z47" s="3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AA47" s="3">
-        <v>14</v>
-      </c>
-      <c r="AB47" s="2">
-        <f>5/127*100000</f>
-        <v>3937.0078740157478</v>
-      </c>
-      <c r="AC47" s="2">
-        <f>14/362*100000</f>
-        <v>3867.4033149171269</v>
+        <v>38</v>
       </c>
       <c r="AD47" s="6">
-        <v>64.900000000000006</v>
+        <v>81.599999999999994</v>
       </c>
       <c r="AE47" s="6">
-        <v>2.5</v>
+        <v>58.8</v>
       </c>
       <c r="AF47" s="6">
-        <v>87.3</v>
+        <v>91.8</v>
       </c>
       <c r="AG47" s="3">
         <v>95</v>
@@ -5647,7 +5625,7 @@
         <v>304</v>
       </c>
       <c r="I48">
-        <v>5</v>
+        <v>0.75</v>
       </c>
       <c r="J48">
         <v>15</v>
@@ -5665,13 +5643,13 @@
         <v>279</v>
       </c>
       <c r="O48" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="P48" s="1" t="s">
         <v>58</v>
       </c>
       <c r="Q48" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="R48" s="1" t="s">
         <v>226</v>
@@ -5683,7 +5661,7 @@
         <v>166</v>
       </c>
       <c r="U48" s="1" t="s">
-        <v>62</v>
+        <v>167</v>
       </c>
       <c r="V48">
         <v>1</v>
@@ -5691,28 +5669,32 @@
       <c r="W48">
         <v>24</v>
       </c>
+      <c r="X48" s="2">
+        <v>10005</v>
+      </c>
+      <c r="Y48" s="2">
+        <v>10014</v>
+      </c>
       <c r="Z48" s="3">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="AA48" s="3">
-        <v>47</v>
-      </c>
-      <c r="AB48" s="2">
-        <f>6/46*100000</f>
-        <v>13043.478260869564</v>
-      </c>
-      <c r="AC48" s="2">
-        <f>47/369*100000</f>
-        <v>12737.127371273713</v>
+        <v>62</v>
+      </c>
+      <c r="AB48" s="3">
+        <v>18145</v>
+      </c>
+      <c r="AC48" s="3">
+        <v>18154</v>
       </c>
       <c r="AD48" s="6">
-        <v>87.5</v>
+        <v>79</v>
       </c>
       <c r="AE48" s="6">
-        <v>70.8</v>
+        <v>61.9</v>
       </c>
       <c r="AF48" s="6">
-        <v>94.5</v>
+        <v>88.5</v>
       </c>
       <c r="AG48" s="3">
         <v>95</v>
@@ -5747,7 +5729,7 @@
         <v>2</v>
       </c>
       <c r="J49">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="K49" s="1" t="s">
         <v>11</v>
@@ -5759,10 +5741,10 @@
         <v>17</v>
       </c>
       <c r="N49" s="1" t="s">
-        <v>298</v>
+        <v>279</v>
       </c>
       <c r="O49" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="P49" s="1" t="s">
         <v>58</v>
@@ -5777,39 +5759,39 @@
         <v>25</v>
       </c>
       <c r="T49" s="1" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="U49" s="1" t="s">
-        <v>168</v>
+        <v>307</v>
       </c>
       <c r="V49">
         <v>1</v>
       </c>
       <c r="W49">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="Z49" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AA49" s="3">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="AB49" s="2">
-        <f>6/61*100000</f>
-        <v>9836.065573770491</v>
+        <f>5/127*100000</f>
+        <v>3937.0078740157478</v>
       </c>
       <c r="AC49" s="2">
-        <f>36/370*100000</f>
-        <v>9729.72972972973</v>
+        <f>14/362*100000</f>
+        <v>3867.4033149171269</v>
       </c>
       <c r="AD49" s="6">
-        <v>83.4</v>
+        <v>64.900000000000006</v>
       </c>
       <c r="AE49" s="6">
-        <v>60.5</v>
+        <v>2.5</v>
       </c>
       <c r="AF49" s="6">
-        <v>93</v>
+        <v>87.3</v>
       </c>
       <c r="AG49" s="3">
         <v>95</v>
@@ -5841,7 +5823,7 @@
         <v>304</v>
       </c>
       <c r="I50">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J50">
         <v>15</v>
@@ -5856,10 +5838,10 @@
         <v>17</v>
       </c>
       <c r="N50" s="1" t="s">
-        <v>298</v>
+        <v>279</v>
       </c>
       <c r="O50" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="P50" s="1" t="s">
         <v>58</v>
@@ -5874,250 +5856,236 @@
         <v>25</v>
       </c>
       <c r="T50" s="1" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="U50" s="1" t="s">
-        <v>168</v>
+        <v>62</v>
       </c>
       <c r="V50">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="W50">
         <v>24</v>
       </c>
       <c r="Z50" s="3">
+        <v>6</v>
+      </c>
+      <c r="AA50" s="3">
+        <v>47</v>
+      </c>
+      <c r="AB50" s="2">
+        <f>6/46*100000</f>
+        <v>13043.478260869564</v>
+      </c>
+      <c r="AC50" s="2">
+        <f>47/369*100000</f>
+        <v>12737.127371273713</v>
+      </c>
+      <c r="AD50" s="6">
+        <v>87.5</v>
+      </c>
+      <c r="AE50" s="6">
+        <v>70.8</v>
+      </c>
+      <c r="AF50" s="6">
+        <v>94.5</v>
+      </c>
+      <c r="AG50" s="3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="51" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B51" t="s">
+        <v>237</v>
+      </c>
+      <c r="C51">
+        <v>2021</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="I51">
+        <v>2</v>
+      </c>
+      <c r="J51">
+        <v>15</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L51" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M51" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N51" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="O51" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="P51" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q51" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="R51" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="S51" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="T51" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="U51" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="V51">
+        <v>1</v>
+      </c>
+      <c r="W51">
+        <v>12</v>
+      </c>
+      <c r="Z51" s="3">
+        <v>6</v>
+      </c>
+      <c r="AA51" s="3">
+        <v>36</v>
+      </c>
+      <c r="AB51" s="2">
+        <f>6/61*100000</f>
+        <v>9836.065573770491</v>
+      </c>
+      <c r="AC51" s="2">
+        <f>36/370*100000</f>
+        <v>9729.72972972973</v>
+      </c>
+      <c r="AD51" s="6">
+        <v>83.4</v>
+      </c>
+      <c r="AE51" s="6">
+        <v>60.5</v>
+      </c>
+      <c r="AF51" s="6">
+        <v>93</v>
+      </c>
+      <c r="AG51" s="3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="52" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B52" t="s">
+        <v>237</v>
+      </c>
+      <c r="C52">
+        <v>2021</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="I52">
+        <v>2</v>
+      </c>
+      <c r="J52">
+        <v>15</v>
+      </c>
+      <c r="K52" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L52" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M52" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N52" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="O52" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="P52" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q52" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="R52" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="S52" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="T52" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="U52" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="V52">
+        <v>13</v>
+      </c>
+      <c r="W52">
+        <v>24</v>
+      </c>
+      <c r="Z52" s="3">
         <v>7</v>
       </c>
-      <c r="AA50" s="3">
+      <c r="AA52" s="3">
         <v>26</v>
       </c>
-      <c r="AB50" s="2">
+      <c r="AB52" s="2">
         <f>7/83*100000</f>
         <v>8433.7349397590351</v>
       </c>
-      <c r="AC50" s="2">
+      <c r="AC52" s="2">
         <f>26/310*100000</f>
         <v>8387.0967741935492</v>
       </c>
-      <c r="AD50" s="6">
+      <c r="AD52" s="6">
         <v>73</v>
       </c>
-      <c r="AE50" s="6">
+      <c r="AE52" s="6">
         <v>37.9</v>
       </c>
-      <c r="AF50" s="6">
+      <c r="AF52" s="6">
         <v>88.3</v>
-      </c>
-      <c r="AG50" s="3">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="51" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A51" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="H51" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="I51" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="J51" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="K51" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L51" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M51" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="N51" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="O51" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="P51" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q51" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="R51" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="S51" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="T51" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="U51" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="V51">
-        <v>18</v>
-      </c>
-      <c r="W51">
-        <v>24</v>
-      </c>
-      <c r="X51" s="2">
-        <v>13945</v>
-      </c>
-      <c r="Y51" s="2">
-        <v>13937</v>
-      </c>
-      <c r="Z51" s="3">
-        <v>10</v>
-      </c>
-      <c r="AA51" s="3">
-        <v>61</v>
-      </c>
-      <c r="AB51" s="3">
-        <v>25323</v>
-      </c>
-      <c r="AC51" s="3">
-        <v>25239</v>
-      </c>
-      <c r="AD51" s="6">
-        <v>83.7</v>
-      </c>
-      <c r="AE51" s="6">
-        <v>68.099999999999994</v>
-      </c>
-      <c r="AF51" s="6">
-        <v>91.6</v>
-      </c>
-      <c r="AG51" s="3">
-        <v>95</v>
-      </c>
-      <c r="AH51" s="1" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="52" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="H52" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="I52" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="J52" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="K52" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L52" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M52" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="N52" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="O52" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="P52" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q52" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="R52" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="S52" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="T52" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="U52" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="V52">
-        <v>18</v>
-      </c>
-      <c r="W52">
-        <v>24</v>
-      </c>
-      <c r="X52" s="2">
-        <v>5044</v>
-      </c>
-      <c r="Y52" s="2">
-        <v>5158</v>
-      </c>
-      <c r="Z52" s="3">
-        <v>5</v>
-      </c>
-      <c r="AA52" s="3">
-        <v>20</v>
-      </c>
-      <c r="AB52" s="3">
-        <v>9057</v>
-      </c>
-      <c r="AC52" s="3">
-        <v>9261</v>
-      </c>
-      <c r="AD52" s="6">
-        <v>74.400000000000006</v>
-      </c>
-      <c r="AE52" s="6">
-        <v>31.8</v>
-      </c>
-      <c r="AF52" s="6">
-        <v>90.4</v>
       </c>
       <c r="AG52" s="3">
         <v>95</v>
-      </c>
-      <c r="AH52" s="1" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="53" spans="1:34" x14ac:dyDescent="0.2">
@@ -6146,7 +6114,7 @@
         <v>304</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>63</v>
+        <v>152</v>
       </c>
       <c r="J53" s="1" t="s">
         <v>65</v>
@@ -6163,14 +6131,14 @@
       <c r="N53" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="O53" s="9" t="s">
-        <v>301</v>
+      <c r="O53" s="1" t="s">
+        <v>300</v>
       </c>
       <c r="P53" s="1" t="s">
         <v>58</v>
       </c>
       <c r="Q53" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="R53" s="1" t="s">
         <v>226</v>
@@ -6182,7 +6150,7 @@
         <v>166</v>
       </c>
       <c r="U53" s="1" t="s">
-        <v>65</v>
+        <v>308</v>
       </c>
       <c r="V53">
         <v>18</v>
@@ -6191,31 +6159,31 @@
         <v>24</v>
       </c>
       <c r="X53" s="2">
-        <v>8901</v>
+        <v>13945</v>
       </c>
       <c r="Y53" s="2">
-        <v>8799</v>
+        <v>13937</v>
       </c>
       <c r="Z53" s="3">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="AA53" s="3">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="AB53" s="3">
-        <v>16267</v>
+        <v>25323</v>
       </c>
       <c r="AC53" s="3">
-        <v>15978</v>
+        <v>25239</v>
       </c>
       <c r="AD53" s="6">
-        <v>88</v>
+        <v>83.7</v>
       </c>
       <c r="AE53" s="6">
-        <v>69.7</v>
+        <v>68.099999999999994</v>
       </c>
       <c r="AF53" s="6">
-        <v>95.3</v>
+        <v>91.6</v>
       </c>
       <c r="AG53" s="3">
         <v>95</v>
@@ -6226,16 +6194,16 @@
     </row>
     <row r="54" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>142</v>
+        <v>269</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>240</v>
@@ -6253,7 +6221,7 @@
         <v>152</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K54" s="1" t="s">
         <v>11</v>
@@ -6265,13 +6233,13 @@
         <v>17</v>
       </c>
       <c r="N54" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="O54" s="1" t="s">
-        <v>300</v>
+        <v>279</v>
+      </c>
+      <c r="O54" s="9" t="s">
+        <v>301</v>
       </c>
       <c r="P54" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="Q54" s="1" t="s">
         <v>144</v>
@@ -6283,63 +6251,63 @@
         <v>25</v>
       </c>
       <c r="T54" s="1" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="U54" s="1" t="s">
-        <v>264</v>
+        <v>65</v>
       </c>
       <c r="V54">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="W54">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="X54" s="2">
-        <v>14069</v>
+        <v>5044</v>
       </c>
       <c r="Y54" s="2">
-        <v>14061</v>
+        <v>5158</v>
       </c>
       <c r="Z54" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AA54" s="3">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="AB54" s="3">
-        <v>14058</v>
+        <v>9057</v>
       </c>
       <c r="AC54" s="3">
-        <v>14046</v>
+        <v>9261</v>
       </c>
       <c r="AD54" s="6">
-        <v>83.4</v>
+        <v>74.400000000000006</v>
       </c>
       <c r="AE54" s="6">
-        <v>60.1</v>
+        <v>31.8</v>
       </c>
       <c r="AF54" s="6">
-        <v>94.3</v>
+        <v>90.4</v>
       </c>
       <c r="AG54" s="3">
         <v>95</v>
       </c>
       <c r="AH54" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="55" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>142</v>
+        <v>269</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>240</v>
@@ -6354,7 +6322,7 @@
         <v>304</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>152</v>
+        <v>63</v>
       </c>
       <c r="J55" s="1" t="s">
         <v>65</v>
@@ -6369,13 +6337,13 @@
         <v>17</v>
       </c>
       <c r="N55" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="O55" s="1" t="s">
-        <v>300</v>
+        <v>279</v>
+      </c>
+      <c r="O55" s="9" t="s">
+        <v>301</v>
       </c>
       <c r="P55" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="Q55" s="1" t="s">
         <v>144</v>
@@ -6387,49 +6355,49 @@
         <v>25</v>
       </c>
       <c r="T55" s="1" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="U55" s="1" t="s">
-        <v>264</v>
+        <v>65</v>
       </c>
       <c r="V55">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="W55">
         <v>24</v>
       </c>
       <c r="X55" s="2">
-        <v>14050</v>
+        <v>8901</v>
       </c>
       <c r="Y55" s="2">
-        <v>14006</v>
+        <v>8799</v>
       </c>
       <c r="Z55" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AA55" s="3">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="AB55" s="3">
-        <v>14046</v>
+        <v>16267</v>
       </c>
       <c r="AC55" s="3">
-        <v>13985</v>
+        <v>15978</v>
       </c>
       <c r="AD55" s="6">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="AE55" s="6">
-        <v>42.9</v>
+        <v>69.7</v>
       </c>
       <c r="AF55" s="6">
-        <v>92.3</v>
+        <v>95.3</v>
       </c>
       <c r="AG55" s="3">
         <v>95</v>
       </c>
       <c r="AH55" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="56" spans="1:34" x14ac:dyDescent="0.2">
@@ -6491,43 +6459,43 @@
         <v>25</v>
       </c>
       <c r="T56" s="1" t="s">
-        <v>274</v>
+        <v>160</v>
       </c>
       <c r="U56" s="1" t="s">
         <v>264</v>
       </c>
       <c r="V56">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="W56">
+        <v>12</v>
+      </c>
+      <c r="X56" s="2">
+        <v>14069</v>
+      </c>
+      <c r="Y56" s="2">
+        <v>14061</v>
+      </c>
+      <c r="Z56" s="3">
+        <v>6</v>
+      </c>
+      <c r="AA56" s="3">
         <v>36</v>
       </c>
-      <c r="X56" s="2">
-        <v>14043</v>
-      </c>
-      <c r="Y56" s="2">
-        <v>13976</v>
-      </c>
-      <c r="Z56" s="3">
-        <v>3</v>
-      </c>
-      <c r="AA56" s="3">
-        <v>139</v>
-      </c>
       <c r="AB56" s="3">
-        <v>14031</v>
+        <v>14058</v>
       </c>
       <c r="AC56" s="3">
-        <v>13963</v>
+        <v>14046</v>
       </c>
       <c r="AD56" s="6">
-        <v>77</v>
+        <v>83.4</v>
       </c>
       <c r="AE56" s="6">
-        <v>16.399999999999999</v>
+        <v>60.1</v>
       </c>
       <c r="AF56" s="6">
-        <v>95.8</v>
+        <v>94.3</v>
       </c>
       <c r="AG56" s="3">
         <v>95</v>
@@ -6595,43 +6563,43 @@
         <v>25</v>
       </c>
       <c r="T57" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="U57" s="1" t="s">
         <v>264</v>
       </c>
       <c r="V57">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="W57">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="X57" s="2">
-        <v>13996</v>
+        <v>14050</v>
       </c>
       <c r="Y57" s="2">
-        <v>13928</v>
+        <v>14006</v>
       </c>
       <c r="Z57" s="3">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="AA57" s="3">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AB57" s="3">
-        <v>13968</v>
+        <v>14046</v>
       </c>
       <c r="AC57" s="3">
-        <v>13906</v>
+        <v>13985</v>
       </c>
       <c r="AD57" s="6">
-        <v>68.2</v>
+        <v>77</v>
       </c>
       <c r="AE57" s="6">
-        <v>27.2</v>
+        <v>42.9</v>
       </c>
       <c r="AF57" s="6">
-        <v>87.6</v>
+        <v>92.3</v>
       </c>
       <c r="AG57" s="3">
         <v>95</v>
@@ -6699,43 +6667,43 @@
         <v>25</v>
       </c>
       <c r="T58" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="U58" s="1" t="s">
         <v>264</v>
       </c>
       <c r="V58">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="W58">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="X58" s="2">
-        <v>13980</v>
+        <v>14043</v>
       </c>
       <c r="Y58" s="2">
-        <v>13893</v>
+        <v>13976</v>
       </c>
       <c r="Z58" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AA58" s="3">
-        <v>10</v>
+        <v>139</v>
       </c>
       <c r="AB58" s="3">
-        <v>4379</v>
+        <v>14031</v>
       </c>
       <c r="AC58" s="3">
-        <v>4331</v>
+        <v>13963</v>
       </c>
       <c r="AD58" s="6">
-        <v>90.1</v>
+        <v>77</v>
       </c>
       <c r="AE58" s="6">
-        <v>30.5</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="AF58" s="6">
-        <v>99.8</v>
+        <v>95.8</v>
       </c>
       <c r="AG58" s="3">
         <v>95</v>
@@ -6773,7 +6741,7 @@
         <v>152</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="K59" s="1" t="s">
         <v>11</v>
@@ -6785,10 +6753,10 @@
         <v>17</v>
       </c>
       <c r="N59" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="O59" s="9" t="s">
-        <v>301</v>
+        <v>298</v>
+      </c>
+      <c r="O59" s="1" t="s">
+        <v>300</v>
       </c>
       <c r="P59" s="1" t="s">
         <v>64</v>
@@ -6803,49 +6771,49 @@
         <v>25</v>
       </c>
       <c r="T59" s="1" t="s">
-        <v>278</v>
+        <v>162</v>
       </c>
       <c r="U59" s="1" t="s">
-        <v>169</v>
+        <v>264</v>
       </c>
       <c r="V59">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="W59">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="X59" s="2">
-        <v>1555</v>
+        <v>13996</v>
       </c>
       <c r="Y59" s="2">
-        <v>1600</v>
+        <v>13928</v>
       </c>
       <c r="Z59" s="3">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="AA59" s="3">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="AB59" s="3">
-        <v>6586</v>
+        <v>13968</v>
       </c>
       <c r="AC59" s="3">
-        <v>6773</v>
+        <v>13906</v>
       </c>
       <c r="AD59" s="6">
-        <v>70.599999999999994</v>
+        <v>68.2</v>
       </c>
       <c r="AE59" s="6">
-        <v>6.4</v>
+        <v>27.2</v>
       </c>
       <c r="AF59" s="6">
-        <v>93</v>
+        <v>87.6</v>
       </c>
       <c r="AG59" s="3">
         <v>95</v>
       </c>
       <c r="AH59" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="60" spans="1:34" x14ac:dyDescent="0.2">
@@ -6874,10 +6842,10 @@
         <v>304</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>59</v>
+        <v>152</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="K60" s="1" t="s">
         <v>11</v>
@@ -6889,10 +6857,10 @@
         <v>17</v>
       </c>
       <c r="N60" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="O60" s="9" t="s">
-        <v>301</v>
+        <v>298</v>
+      </c>
+      <c r="O60" s="1" t="s">
+        <v>300</v>
       </c>
       <c r="P60" s="1" t="s">
         <v>64</v>
@@ -6907,49 +6875,49 @@
         <v>25</v>
       </c>
       <c r="T60" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="U60" s="1" t="s">
-        <v>169</v>
+        <v>264</v>
       </c>
       <c r="V60">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="W60">
         <v>55</v>
       </c>
       <c r="X60" s="2">
-        <v>3503</v>
+        <v>13980</v>
       </c>
       <c r="Y60" s="2">
-        <v>3579</v>
+        <v>13893</v>
       </c>
       <c r="Z60" s="3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AA60" s="3">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="AB60" s="3">
-        <v>15007</v>
+        <v>4379</v>
       </c>
       <c r="AC60" s="3">
-        <v>15297</v>
+        <v>4331</v>
       </c>
       <c r="AD60" s="6">
-        <v>79.599999999999994</v>
+        <v>90.1</v>
       </c>
       <c r="AE60" s="6">
-        <v>45.8</v>
+        <v>30.5</v>
       </c>
       <c r="AF60" s="6">
-        <v>93.9</v>
+        <v>99.8</v>
       </c>
       <c r="AG60" s="3">
         <v>95</v>
       </c>
       <c r="AH60" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="61" spans="1:34" x14ac:dyDescent="0.2">
@@ -6978,10 +6946,10 @@
         <v>304</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>63</v>
+        <v>152</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="K61" s="1" t="s">
         <v>11</v>
@@ -7023,31 +6991,31 @@
         <v>55</v>
       </c>
       <c r="X61" s="2">
-        <v>9011</v>
+        <v>1555</v>
       </c>
       <c r="Y61" s="2">
-        <v>8882</v>
+        <v>1600</v>
       </c>
       <c r="Z61" s="3">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="AA61" s="3">
-        <v>71</v>
+        <v>14</v>
       </c>
       <c r="AB61" s="3">
-        <v>38907</v>
+        <v>6586</v>
       </c>
       <c r="AC61" s="3">
-        <v>38151</v>
+        <v>6773</v>
       </c>
       <c r="AD61" s="6">
-        <v>79.3</v>
+        <v>70.599999999999994</v>
       </c>
       <c r="AE61" s="6">
-        <v>63.5</v>
+        <v>6.4</v>
       </c>
       <c r="AF61" s="6">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="AG61" s="3">
         <v>95</v>
@@ -7079,13 +7047,13 @@
         <v>271</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>152</v>
+        <v>59</v>
       </c>
       <c r="J62" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K62" s="1" t="s">
         <v>11</v>
@@ -7099,14 +7067,14 @@
       <c r="N62" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="O62" s="1" t="s">
-        <v>300</v>
+      <c r="O62" s="9" t="s">
+        <v>301</v>
       </c>
       <c r="P62" s="1" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="Q62" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="R62" s="1" t="s">
         <v>226</v>
@@ -7118,7 +7086,7 @@
         <v>278</v>
       </c>
       <c r="U62" s="1" t="s">
-        <v>153</v>
+        <v>169</v>
       </c>
       <c r="V62">
         <v>1</v>
@@ -7127,37 +7095,37 @@
         <v>55</v>
       </c>
       <c r="X62" s="2">
-        <v>14069</v>
+        <v>3503</v>
       </c>
       <c r="Y62" s="2">
-        <v>14061</v>
+        <v>3579</v>
       </c>
       <c r="Z62" s="3">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="AA62" s="3">
-        <v>110</v>
+        <v>25</v>
       </c>
       <c r="AB62" s="3">
-        <v>60500</v>
+        <v>15007</v>
       </c>
       <c r="AC62" s="3">
-        <v>60220</v>
+        <v>15297</v>
       </c>
       <c r="AD62" s="6">
-        <v>78.3</v>
+        <v>79.599999999999994</v>
       </c>
       <c r="AE62" s="6">
-        <v>66.3</v>
+        <v>45.8</v>
       </c>
       <c r="AF62" s="6">
-        <v>86.1</v>
+        <v>93.9</v>
       </c>
       <c r="AG62" s="3">
         <v>95</v>
       </c>
       <c r="AH62" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="63" spans="1:34" x14ac:dyDescent="0.2">
@@ -7183,10 +7151,10 @@
         <v>271</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>276</v>
+        <v>304</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>152</v>
+        <v>63</v>
       </c>
       <c r="J63" s="1" t="s">
         <v>65</v>
@@ -7203,14 +7171,14 @@
       <c r="N63" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="O63" s="1" t="s">
-        <v>300</v>
+      <c r="O63" s="9" t="s">
+        <v>301</v>
       </c>
       <c r="P63" s="1" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="Q63" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="R63" s="1" t="s">
         <v>226</v>
@@ -7222,7 +7190,7 @@
         <v>278</v>
       </c>
       <c r="U63" s="1" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="V63">
         <v>1</v>
@@ -7231,69 +7199,69 @@
         <v>55</v>
       </c>
       <c r="X63" s="2">
-        <v>13945</v>
+        <v>9011</v>
       </c>
       <c r="Y63" s="2">
-        <v>13937</v>
+        <v>8882</v>
       </c>
       <c r="Z63" s="3">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="AA63" s="3">
-        <v>109</v>
+        <v>71</v>
       </c>
       <c r="AB63" s="3">
-        <v>59942</v>
+        <v>38907</v>
       </c>
       <c r="AC63" s="3">
-        <v>59662</v>
+        <v>38151</v>
       </c>
       <c r="AD63" s="6">
-        <v>80</v>
+        <v>79.3</v>
       </c>
       <c r="AE63" s="6">
-        <v>68.3</v>
+        <v>63.5</v>
       </c>
       <c r="AF63" s="6">
-        <v>87.3</v>
+        <v>89</v>
       </c>
       <c r="AG63" s="3">
         <v>95</v>
       </c>
       <c r="AH63" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="64" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>283</v>
+        <v>266</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>267</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>284</v>
+        <v>142</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>289</v>
+        <v>272</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>285</v>
+        <v>240</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>286</v>
+        <v>13</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>288</v>
+        <v>271</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>59</v>
+        <v>152</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="K64" s="1" t="s">
         <v>11</v>
@@ -7307,7 +7275,7 @@
       <c r="N64" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="O64" s="9" t="s">
+      <c r="O64" s="1" t="s">
         <v>300</v>
       </c>
       <c r="P64" s="1" t="s">
@@ -7320,75 +7288,84 @@
         <v>226</v>
       </c>
       <c r="S64" s="1" t="s">
-        <v>291</v>
+        <v>25</v>
       </c>
       <c r="T64" s="1" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="U64" s="1" t="s">
-        <v>309</v>
+        <v>153</v>
       </c>
       <c r="V64">
         <v>1</v>
       </c>
       <c r="W64">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="X64" s="2">
-        <v>5525</v>
+        <v>14069</v>
       </c>
       <c r="Y64" s="2">
-        <v>5566</v>
+        <v>14061</v>
       </c>
       <c r="Z64" s="3">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="AA64" s="3">
-        <v>47</v>
+        <v>110</v>
+      </c>
+      <c r="AB64" s="3">
+        <v>60500</v>
+      </c>
+      <c r="AC64" s="3">
+        <v>60220</v>
       </c>
       <c r="AD64" s="6">
-        <v>91.5</v>
+        <v>78.3</v>
       </c>
       <c r="AE64" s="6">
-        <v>77.099999999999994</v>
+        <v>66.3</v>
       </c>
       <c r="AF64" s="6">
-        <v>96.6</v>
+        <v>86.1</v>
       </c>
       <c r="AG64" s="3">
         <v>95</v>
       </c>
+      <c r="AH64" s="1" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="65" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>283</v>
+        <v>266</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>267</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>284</v>
+        <v>142</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>289</v>
+        <v>272</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>285</v>
+        <v>240</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>288</v>
+        <v>271</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>304</v>
+        <v>276</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>59</v>
+        <v>152</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="K65" s="1" t="s">
         <v>11</v>
@@ -7402,7 +7379,7 @@
       <c r="N65" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="O65" s="9" t="s">
+      <c r="O65" s="1" t="s">
         <v>300</v>
       </c>
       <c r="P65" s="1" t="s">
@@ -7415,46 +7392,52 @@
         <v>226</v>
       </c>
       <c r="S65" s="1" t="s">
-        <v>291</v>
+        <v>25</v>
       </c>
       <c r="T65" s="1" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="U65" s="1" t="s">
-        <v>148</v>
+        <v>164</v>
       </c>
       <c r="V65">
         <v>1</v>
       </c>
       <c r="W65">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="X65" s="2">
-        <v>378</v>
+        <v>13945</v>
       </c>
       <c r="Y65" s="2">
-        <v>393</v>
+        <v>13937</v>
       </c>
       <c r="Z65" s="3">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="AA65" s="3">
-        <v>8</v>
+        <v>109</v>
+      </c>
+      <c r="AB65" s="3">
+        <v>59942</v>
+      </c>
+      <c r="AC65" s="3">
+        <v>59662</v>
       </c>
       <c r="AD65" s="6">
-        <v>87.7</v>
+        <v>80</v>
       </c>
       <c r="AE65" s="6">
-        <v>3.8</v>
+        <v>68.3</v>
       </c>
       <c r="AF65" s="6">
-        <v>99.7</v>
+        <v>87.3</v>
       </c>
       <c r="AG65" s="3">
         <v>95</v>
       </c>
       <c r="AH65" s="1" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
     </row>
     <row r="66" spans="1:34" x14ac:dyDescent="0.2">
@@ -7489,7 +7472,7 @@
         <v>63</v>
       </c>
       <c r="K66" s="1" t="s">
-        <v>292</v>
+        <v>11</v>
       </c>
       <c r="L66" s="1" t="s">
         <v>21</v>
@@ -7504,7 +7487,7 @@
         <v>300</v>
       </c>
       <c r="P66" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="Q66" s="1" t="s">
         <v>145</v>
@@ -7528,27 +7511,220 @@
         <v>27</v>
       </c>
       <c r="X66" s="2">
-        <v>5</v>
+        <v>5525</v>
       </c>
       <c r="Y66" s="2">
+        <v>5566</v>
+      </c>
+      <c r="Z66" s="3">
+        <v>4</v>
+      </c>
+      <c r="AA66" s="3">
+        <v>47</v>
+      </c>
+      <c r="AD66" s="6">
+        <v>91.5</v>
+      </c>
+      <c r="AE66" s="6">
+        <v>77.099999999999994</v>
+      </c>
+      <c r="AF66" s="6">
+        <v>96.6</v>
+      </c>
+      <c r="AG66" s="3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="67" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="I67" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J67" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K67" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L67" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M67" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N67" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="O67" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="P67" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q67" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="R67" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="S67" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="T67" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="U67" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="V67">
+        <v>1</v>
+      </c>
+      <c r="W67">
+        <v>27</v>
+      </c>
+      <c r="X67" s="2">
+        <v>378</v>
+      </c>
+      <c r="Y67" s="2">
+        <v>393</v>
+      </c>
+      <c r="Z67" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA67" s="3">
+        <v>8</v>
+      </c>
+      <c r="AD67" s="6">
+        <v>87.7</v>
+      </c>
+      <c r="AE67" s="6">
+        <v>3.8</v>
+      </c>
+      <c r="AF67" s="6">
+        <v>99.7</v>
+      </c>
+      <c r="AG67" s="3">
+        <v>95</v>
+      </c>
+      <c r="AH67" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="68" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="I68" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J68" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K68" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="L68" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M68" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N68" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="O68" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="P68" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q68" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="R68" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="S68" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="T68" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="U68" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="V68">
+        <v>1</v>
+      </c>
+      <c r="W68">
+        <v>27</v>
+      </c>
+      <c r="X68" s="2">
+        <v>5</v>
+      </c>
+      <c r="Y68" s="2">
         <v>56</v>
       </c>
-      <c r="Z66" s="3">
+      <c r="Z68" s="3">
         <v>0</v>
       </c>
-      <c r="AA66" s="3">
+      <c r="AA68" s="3">
         <v>21</v>
       </c>
-      <c r="AD66" s="6">
+      <c r="AD68" s="6">
         <v>100</v>
       </c>
-      <c r="AE66" s="6">
+      <c r="AE68" s="6">
         <v>-102</v>
       </c>
-      <c r="AF66" s="6">
+      <c r="AF68" s="6">
         <v>100</v>
       </c>
-      <c r="AG66" s="3">
+      <c r="AG68" s="3">
         <v>95</v>
       </c>
     </row>
@@ -7556,21 +7732,22 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B17" r:id="rId1" xr:uid="{161F70B6-3FFB-634B-99FC-3B4164591F9E}"/>
-    <hyperlink ref="B52" r:id="rId2" xr:uid="{7FC01869-90C0-5644-8714-26700C8CC743}"/>
-    <hyperlink ref="B53" r:id="rId3" xr:uid="{F9ADD7E8-AA8D-4748-9EFC-6348B4B74A9E}"/>
-    <hyperlink ref="B51" r:id="rId4" xr:uid="{DABF1983-39B7-5042-9E81-1088839BA79E}"/>
-    <hyperlink ref="B54" r:id="rId5" xr:uid="{1BC27440-E48F-1344-BAEF-5C2A389E5114}"/>
-    <hyperlink ref="B55" r:id="rId6" xr:uid="{06CF78B3-DBE3-274E-94E8-0A957485B676}"/>
-    <hyperlink ref="B56" r:id="rId7" xr:uid="{40CEFE4D-A3B5-1046-93E2-4196ED0846A2}"/>
-    <hyperlink ref="B57" r:id="rId8" xr:uid="{700D5137-2144-9641-A42A-88D0F68E8522}"/>
-    <hyperlink ref="B58" r:id="rId9" xr:uid="{B1098C8C-4D37-9844-9395-756F0046D696}"/>
-    <hyperlink ref="B59" r:id="rId10" xr:uid="{00C6B523-31EF-5F46-A014-DD8D179224F6}"/>
-    <hyperlink ref="B60" r:id="rId11" xr:uid="{09A83033-79FD-5C4E-A152-CCF436016F9E}"/>
-    <hyperlink ref="B61" r:id="rId12" xr:uid="{4649D6C8-50AE-2346-B248-C037AB4D4A04}"/>
-    <hyperlink ref="B62" r:id="rId13" xr:uid="{ED0C29F5-D24A-F949-8A39-BCD52DCB17E2}"/>
-    <hyperlink ref="B63" r:id="rId14" xr:uid="{A0657EF5-A0C2-B44B-87BD-58CAAB44DFAF}"/>
+    <hyperlink ref="B54" r:id="rId2" xr:uid="{7FC01869-90C0-5644-8714-26700C8CC743}"/>
+    <hyperlink ref="B55" r:id="rId3" xr:uid="{F9ADD7E8-AA8D-4748-9EFC-6348B4B74A9E}"/>
+    <hyperlink ref="B53" r:id="rId4" xr:uid="{DABF1983-39B7-5042-9E81-1088839BA79E}"/>
+    <hyperlink ref="B56" r:id="rId5" xr:uid="{1BC27440-E48F-1344-BAEF-5C2A389E5114}"/>
+    <hyperlink ref="B57" r:id="rId6" xr:uid="{06CF78B3-DBE3-274E-94E8-0A957485B676}"/>
+    <hyperlink ref="B58" r:id="rId7" xr:uid="{40CEFE4D-A3B5-1046-93E2-4196ED0846A2}"/>
+    <hyperlink ref="B59" r:id="rId8" xr:uid="{700D5137-2144-9641-A42A-88D0F68E8522}"/>
+    <hyperlink ref="B60" r:id="rId9" xr:uid="{B1098C8C-4D37-9844-9395-756F0046D696}"/>
+    <hyperlink ref="B61" r:id="rId10" xr:uid="{00C6B523-31EF-5F46-A014-DD8D179224F6}"/>
+    <hyperlink ref="B62" r:id="rId11" xr:uid="{09A83033-79FD-5C4E-A152-CCF436016F9E}"/>
+    <hyperlink ref="B63" r:id="rId12" xr:uid="{4649D6C8-50AE-2346-B248-C037AB4D4A04}"/>
+    <hyperlink ref="B64" r:id="rId13" xr:uid="{ED0C29F5-D24A-F949-8A39-BCD52DCB17E2}"/>
+    <hyperlink ref="B65" r:id="rId14" xr:uid="{A0657EF5-A0C2-B44B-87BD-58CAAB44DFAF}"/>
     <hyperlink ref="B34" r:id="rId15" xr:uid="{5756AE19-E495-984B-84AC-EC614B39B5C2}"/>
     <hyperlink ref="B2" r:id="rId16" xr:uid="{3A085ACA-DCD6-AA41-AA76-20A79D6736A6}"/>
+    <hyperlink ref="B30" r:id="rId17" xr:uid="{07E6818A-27D6-2A42-B101-9BAFBB171B4E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7580,15 +7757,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{149A3A41-8A6C-584E-BBE8-03656533BC7D}">
   <dimension ref="A1:CB33"/>
   <sheetViews>
-    <sheetView topLeftCell="BE1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="AQ1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="BR8" sqref="BR8:BX11"/>
+      <selection pane="bottomLeft" activeCell="AZ5" sqref="AZ5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="10.83203125" style="10"/>
     <col min="4" max="4" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
@@ -7599,7 +7775,7 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" t="s">
         <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -7841,7 +8017,7 @@
       <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="10">
+      <c r="C2">
         <v>2021</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -7963,7 +8139,7 @@
       <c r="B3" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3">
         <v>2024</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -8097,7 +8273,7 @@
       <c r="B4" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4">
         <v>2024</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -8231,7 +8407,7 @@
       <c r="B5" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" t="s">
         <v>142</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -8365,7 +8541,7 @@
       <c r="B6" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" t="s">
         <v>142</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -8499,7 +8675,7 @@
       <c r="B7" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" t="s">
         <v>142</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -8633,7 +8809,7 @@
       <c r="B8" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" t="s">
         <v>142</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -8722,7 +8898,7 @@
       <c r="B9" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" t="s">
         <v>142</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -8811,7 +8987,7 @@
       <c r="B10" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" t="s">
         <v>142</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -8900,7 +9076,7 @@
       <c r="B11" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" t="s">
         <v>142</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -8989,7 +9165,7 @@
       <c r="B12" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12">
         <v>2022</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -9144,7 +9320,7 @@
       <c r="B13" t="s">
         <v>221</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13">
         <v>2017</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -9242,7 +9418,7 @@
       <c r="B14" t="s">
         <v>221</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14">
         <v>2017</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -9337,7 +9513,7 @@
       <c r="B15" t="s">
         <v>237</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15">
         <v>2021</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -9489,7 +9665,7 @@
       <c r="B16" t="s">
         <v>237</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C16">
         <v>2021</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -9641,7 +9817,7 @@
       <c r="B17" t="s">
         <v>237</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C17">
         <v>2021</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -9781,7 +9957,7 @@
       <c r="B18" t="s">
         <v>237</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18">
         <v>2021</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -9918,7 +10094,7 @@
       <c r="B19" t="s">
         <v>237</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C19">
         <v>2021</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -10055,7 +10231,7 @@
       <c r="B20" t="s">
         <v>237</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C20">
         <v>2021</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -10192,7 +10368,7 @@
       <c r="B21" t="s">
         <v>237</v>
       </c>
-      <c r="C21" s="10">
+      <c r="C21">
         <v>2021</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -10329,7 +10505,7 @@
       <c r="B22" t="s">
         <v>237</v>
       </c>
-      <c r="C22" s="10">
+      <c r="C22">
         <v>2021</v>
       </c>
       <c r="D22" s="1" t="s">
@@ -10466,7 +10642,7 @@
       <c r="B23" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" t="s">
         <v>251</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -10546,7 +10722,7 @@
       <c r="B24" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" t="s">
         <v>251</v>
       </c>
       <c r="D24" s="1" t="s">
@@ -10626,7 +10802,7 @@
       <c r="B25" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" t="s">
         <v>251</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -10706,7 +10882,7 @@
       <c r="B26" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" t="s">
         <v>251</v>
       </c>
       <c r="D26" s="1" t="s">
@@ -10786,7 +10962,7 @@
       <c r="B27" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C27" t="s">
         <v>251</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -10866,7 +11042,7 @@
       <c r="B28" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C28" t="s">
         <v>251</v>
       </c>
       <c r="D28" s="1" t="s">
@@ -10946,7 +11122,7 @@
       <c r="B29" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" t="s">
         <v>251</v>
       </c>
       <c r="D29" s="1" t="s">
@@ -11026,7 +11202,7 @@
       <c r="B30" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C30" t="s">
         <v>251</v>
       </c>
       <c r="D30" s="1" t="s">
@@ -11106,7 +11282,7 @@
       <c r="B31" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C31" t="s">
         <v>251</v>
       </c>
       <c r="D31" s="1" t="s">
@@ -11168,7 +11344,7 @@
       <c r="B32" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="C32" t="s">
         <v>251</v>
       </c>
       <c r="D32" s="1" t="s">
@@ -11230,7 +11406,7 @@
       <c r="B33" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C33" t="s">
         <v>251</v>
       </c>
       <c r="D33" s="1" t="s">

</xml_diff>

<commit_message>
tons of model prototyping. Garbage code but hey. - full run through of waning, VE, and boosting - point estimate fits and model - no documentation yet
</commit_message>
<xml_diff>
--- a/data/typhoid_vaccine_study_data.xlsx
+++ b/data/typhoid_vaccine_study_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/famulare/git/famulare/typhoid-immune-dynamics/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFFE34F2-5E76-4E4A-9E65-8E8FBE73A170}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{756D3408-FE89-9941-9A7F-22F89B23DB33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="840" windowWidth="33600" windowHeight="17440" xr2:uid="{3C28E045-1CB7-C04C-9830-A174AB0F25A4}"/>
+    <workbookView xWindow="20060" yWindow="840" windowWidth="14500" windowHeight="17440" activeTab="1" xr2:uid="{3C28E045-1CB7-C04C-9830-A174AB0F25A4}"/>
   </bookViews>
   <sheets>
     <sheet name="efficacy" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2897" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3033" uniqueCount="326">
   <si>
     <t>study</t>
   </si>
@@ -974,6 +974,51 @@
   </si>
   <si>
     <t>fever&gt;=38</t>
+  </si>
+  <si>
+    <t>Kossaczka1999</t>
+  </si>
+  <si>
+    <t>https://pmc.ncbi.nlm.nih.gov/articles/PMC96958/</t>
+  </si>
+  <si>
+    <t>anti_Vi_IgG_Jackson_ImmunoResearch_Laboratories</t>
+  </si>
+  <si>
+    <t>anti_Vi_IgA_HP6107_George_Carlone_CDC</t>
+  </si>
+  <si>
+    <t>treatment_day182_N</t>
+  </si>
+  <si>
+    <t>treatment_day182_seropositive_percent</t>
+  </si>
+  <si>
+    <t>treatment_day182_elisa_U_per_ml_median</t>
+  </si>
+  <si>
+    <t>treatment_day182_elisa_U_per_ml_lower</t>
+  </si>
+  <si>
+    <t>treatment_day182_elisa_U_per_ml_upper</t>
+  </si>
+  <si>
+    <t>Vi-rEPA2</t>
+  </si>
+  <si>
+    <t>treatment_day70_N</t>
+  </si>
+  <si>
+    <t>treatment_day70_seropositive_percent</t>
+  </si>
+  <si>
+    <t>treatment_day70_elisa_U_per_ml_median</t>
+  </si>
+  <si>
+    <t>treatment_day70_elisa_U_per_ml_lower</t>
+  </si>
+  <si>
+    <t>treatment_day70_elisa_U_per_ml_upper</t>
   </si>
 </sst>
 </file>
@@ -1383,9 +1428,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E976F573-8D26-E847-8FB6-13AA5974A482}">
   <dimension ref="A1:AH68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AD44" sqref="AD44"/>
+    <sheetView topLeftCell="A50" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F66" sqref="F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7444,7 +7489,7 @@
       <c r="A66" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B66" s="5" t="s">
         <v>283</v>
       </c>
       <c r="C66" s="1" t="s">
@@ -7748,6 +7793,7 @@
     <hyperlink ref="B34" r:id="rId15" xr:uid="{5756AE19-E495-984B-84AC-EC614B39B5C2}"/>
     <hyperlink ref="B2" r:id="rId16" xr:uid="{3A085ACA-DCD6-AA41-AA76-20A79D6736A6}"/>
     <hyperlink ref="B30" r:id="rId17" xr:uid="{07E6818A-27D6-2A42-B101-9BAFBB171B4E}"/>
+    <hyperlink ref="B66" r:id="rId18" xr:uid="{5EFC5055-71C3-9848-B6B5-7D82010C4DBE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7755,12 +7801,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{149A3A41-8A6C-584E-BBE8-03656533BC7D}">
-  <dimension ref="A1:CB33"/>
+  <dimension ref="A1:CL46"/>
   <sheetViews>
-    <sheetView topLeftCell="AQ1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="AZ5" sqref="AZ5"/>
+      <selection pane="bottomLeft" activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7768,7 +7814,7 @@
     <col min="4" max="4" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:90" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7917,100 +7963,130 @@
         <v>132</v>
       </c>
       <c r="AX1" t="s">
+        <v>321</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>322</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>323</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>324</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>325</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>315</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>316</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>317</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>318</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>319</v>
+      </c>
+      <c r="BH1" t="s">
         <v>185</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="BI1" t="s">
         <v>186</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BJ1" t="s">
         <v>187</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BK1" t="s">
         <v>188</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BL1" t="s">
         <v>189</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BM1" t="s">
         <v>241</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BN1" t="s">
         <v>242</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BO1" t="s">
         <v>243</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BP1" t="s">
         <v>244</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BQ1" t="s">
         <v>245</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BR1" t="s">
         <v>190</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BS1" t="s">
         <v>191</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BT1" t="s">
         <v>192</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BU1" t="s">
         <v>193</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BV1" t="s">
         <v>194</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BW1" t="s">
         <v>213</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BX1" t="s">
         <v>214</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BY1" t="s">
         <v>215</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="BZ1" t="s">
         <v>216</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="CA1" t="s">
         <v>217</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="CB1" t="s">
         <v>195</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="CC1" t="s">
         <v>196</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="CD1" t="s">
         <v>197</v>
       </c>
-      <c r="BU1" t="s">
+      <c r="CE1" t="s">
         <v>198</v>
       </c>
-      <c r="BV1" t="s">
+      <c r="CF1" t="s">
         <v>199</v>
       </c>
-      <c r="BW1" t="s">
+      <c r="CG1" t="s">
         <v>200</v>
       </c>
-      <c r="BX1" t="s">
+      <c r="CH1" t="s">
         <v>201</v>
       </c>
-      <c r="BY1" t="s">
+      <c r="CI1" t="s">
         <v>202</v>
       </c>
-      <c r="BZ1" t="s">
+      <c r="CJ1" t="s">
         <v>203</v>
       </c>
-      <c r="CA1" t="s">
+      <c r="CK1" t="s">
         <v>204</v>
       </c>
-      <c r="CB1" t="s">
+      <c r="CL1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:90" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -8132,7 +8208,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="3" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:90" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>140</v>
       </c>
@@ -8202,21 +8278,6 @@
       <c r="Z3">
         <v>100</v>
       </c>
-      <c r="AX3">
-        <v>15</v>
-      </c>
-      <c r="AY3">
-        <v>93</v>
-      </c>
-      <c r="AZ3">
-        <v>23.14</v>
-      </c>
-      <c r="BA3">
-        <v>12.6</v>
-      </c>
-      <c r="BB3">
-        <v>42.5</v>
-      </c>
       <c r="BH3">
         <v>15</v>
       </c>
@@ -8224,13 +8285,13 @@
         <v>93</v>
       </c>
       <c r="BJ3">
-        <v>18.2</v>
+        <v>23.14</v>
       </c>
       <c r="BK3">
-        <v>8.9</v>
+        <v>12.6</v>
       </c>
       <c r="BL3">
-        <v>37.200000000000003</v>
+        <v>42.5</v>
       </c>
       <c r="BR3">
         <v>15</v>
@@ -8239,34 +8300,49 @@
         <v>93</v>
       </c>
       <c r="BT3">
-        <v>13.4</v>
+        <v>18.2</v>
       </c>
       <c r="BU3">
         <v>8.9</v>
       </c>
       <c r="BV3">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="CB3">
+        <v>15</v>
+      </c>
+      <c r="CC3">
+        <v>93</v>
+      </c>
+      <c r="CD3">
+        <v>13.4</v>
+      </c>
+      <c r="CE3">
+        <v>8.9</v>
+      </c>
+      <c r="CF3">
         <v>20.100000000000001</v>
       </c>
-      <c r="BW3">
-        <v>15</v>
-      </c>
-      <c r="BX3">
+      <c r="CG3">
+        <v>15</v>
+      </c>
+      <c r="CH3">
         <v>87</v>
       </c>
-      <c r="BY3">
+      <c r="CI3">
         <v>10.5</v>
       </c>
-      <c r="BZ3" t="s">
+      <c r="CJ3" t="s">
         <v>119</v>
       </c>
-      <c r="CA3">
+      <c r="CK3">
         <v>14.8</v>
       </c>
-      <c r="CB3" t="s">
+      <c r="CL3" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="4" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:90" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>140</v>
       </c>
@@ -8336,71 +8412,71 @@
       <c r="Z4">
         <v>100</v>
       </c>
-      <c r="AX4">
-        <v>117</v>
-      </c>
-      <c r="AY4">
-        <v>99</v>
-      </c>
-      <c r="AZ4">
-        <v>62.1</v>
-      </c>
-      <c r="BA4">
-        <v>52.1</v>
-      </c>
-      <c r="BB4">
-        <v>74.099999999999994</v>
-      </c>
       <c r="BH4">
         <v>117</v>
       </c>
       <c r="BI4">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BJ4">
-        <v>44.5</v>
+        <v>62.1</v>
       </c>
       <c r="BK4">
-        <v>37.4</v>
+        <v>52.1</v>
       </c>
       <c r="BL4">
-        <v>53</v>
+        <v>74.099999999999994</v>
       </c>
       <c r="BR4">
         <v>117</v>
       </c>
       <c r="BS4">
+        <v>100</v>
+      </c>
+      <c r="BT4">
+        <v>44.5</v>
+      </c>
+      <c r="BU4">
+        <v>37.4</v>
+      </c>
+      <c r="BV4">
+        <v>53</v>
+      </c>
+      <c r="CB4">
+        <v>117</v>
+      </c>
+      <c r="CC4">
         <v>96</v>
       </c>
-      <c r="BT4">
-        <v>28</v>
-      </c>
-      <c r="BU4">
+      <c r="CD4">
+        <v>28</v>
+      </c>
+      <c r="CE4">
         <v>22.3</v>
       </c>
-      <c r="BV4">
+      <c r="CF4">
         <v>35.1</v>
       </c>
-      <c r="BW4">
+      <c r="CG4">
         <v>117</v>
       </c>
-      <c r="BX4">
+      <c r="CH4">
         <v>95</v>
       </c>
-      <c r="BY4">
+      <c r="CI4">
         <v>24.7</v>
       </c>
-      <c r="BZ4">
+      <c r="CJ4">
         <v>19.5</v>
       </c>
-      <c r="CA4">
+      <c r="CK4">
         <v>31.3</v>
       </c>
-      <c r="CB4" t="s">
+      <c r="CL4" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="5" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:90" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>140</v>
       </c>
@@ -8470,71 +8546,71 @@
       <c r="Z5">
         <v>99.5</v>
       </c>
-      <c r="AX5">
-        <v>372</v>
-      </c>
-      <c r="AY5">
-        <v>98.6</v>
-      </c>
-      <c r="AZ5">
-        <v>105</v>
-      </c>
-      <c r="BA5">
-        <v>94</v>
-      </c>
-      <c r="BB5">
-        <v>118</v>
-      </c>
       <c r="BH5">
         <v>372</v>
       </c>
       <c r="BI5">
-        <v>98.9</v>
+        <v>98.6</v>
       </c>
       <c r="BJ5">
-        <v>75</v>
+        <v>105</v>
       </c>
       <c r="BK5">
-        <v>67</v>
+        <v>94</v>
       </c>
       <c r="BL5">
-        <v>84</v>
+        <v>118</v>
       </c>
       <c r="BR5">
         <v>372</v>
       </c>
       <c r="BS5">
+        <v>98.9</v>
+      </c>
+      <c r="BT5">
+        <v>75</v>
+      </c>
+      <c r="BU5">
+        <v>67</v>
+      </c>
+      <c r="BV5">
+        <v>84</v>
+      </c>
+      <c r="CB5">
+        <v>372</v>
+      </c>
+      <c r="CC5">
         <v>98.7</v>
       </c>
-      <c r="BT5">
+      <c r="CD5">
         <v>62</v>
       </c>
-      <c r="BU5">
+      <c r="CE5">
         <v>54</v>
       </c>
-      <c r="BV5">
+      <c r="CF5">
         <v>71</v>
       </c>
-      <c r="BW5">
+      <c r="CG5">
         <v>372</v>
       </c>
-      <c r="BX5">
+      <c r="CH5">
         <v>98.4</v>
       </c>
-      <c r="BY5">
+      <c r="CI5">
         <v>55</v>
       </c>
-      <c r="BZ5">
+      <c r="CJ5">
         <v>48</v>
       </c>
-      <c r="CA5">
+      <c r="CK5">
         <v>63</v>
       </c>
-      <c r="CB5" t="s">
+      <c r="CL5" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="6" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:90" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>140</v>
       </c>
@@ -8604,71 +8680,71 @@
       <c r="Z6">
         <v>100</v>
       </c>
-      <c r="AX6">
-        <v>236</v>
-      </c>
-      <c r="AY6">
-        <v>98.3</v>
-      </c>
-      <c r="AZ6">
-        <v>168</v>
-      </c>
-      <c r="BA6">
-        <v>146</v>
-      </c>
-      <c r="BB6">
-        <v>193</v>
-      </c>
       <c r="BH6">
         <v>236</v>
       </c>
       <c r="BI6">
-        <v>99.1</v>
+        <v>98.3</v>
       </c>
       <c r="BJ6">
-        <v>129</v>
+        <v>168</v>
       </c>
       <c r="BK6">
-        <v>112</v>
+        <v>146</v>
       </c>
       <c r="BL6">
-        <v>149</v>
+        <v>193</v>
       </c>
       <c r="BR6">
         <v>236</v>
       </c>
       <c r="BS6">
+        <v>99.1</v>
+      </c>
+      <c r="BT6">
+        <v>129</v>
+      </c>
+      <c r="BU6">
+        <v>112</v>
+      </c>
+      <c r="BV6">
+        <v>149</v>
+      </c>
+      <c r="CB6">
+        <v>236</v>
+      </c>
+      <c r="CC6">
         <v>99.6</v>
       </c>
-      <c r="BT6">
+      <c r="CD6">
         <v>109</v>
       </c>
-      <c r="BU6">
+      <c r="CE6">
         <v>80</v>
       </c>
-      <c r="BV6">
+      <c r="CF6">
         <v>126</v>
       </c>
-      <c r="BW6">
+      <c r="CG6">
         <v>236</v>
       </c>
-      <c r="BX6">
+      <c r="CH6">
         <v>99.6</v>
       </c>
-      <c r="BY6">
+      <c r="CI6">
         <v>93</v>
       </c>
-      <c r="BZ6">
+      <c r="CJ6">
         <v>80</v>
       </c>
-      <c r="CA6">
+      <c r="CK6">
         <v>109</v>
       </c>
-      <c r="CB6" t="s">
+      <c r="CL6" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="7" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:90" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>140</v>
       </c>
@@ -8738,35 +8814,20 @@
       <c r="Z7">
         <v>99.2</v>
       </c>
-      <c r="AX7">
-        <v>269</v>
-      </c>
-      <c r="AY7">
-        <v>99.2</v>
-      </c>
-      <c r="AZ7">
-        <v>230</v>
-      </c>
-      <c r="BA7">
-        <v>201</v>
-      </c>
-      <c r="BB7">
-        <v>263</v>
-      </c>
       <c r="BH7">
         <v>269</v>
       </c>
       <c r="BI7">
-        <v>99.6</v>
+        <v>99.2</v>
       </c>
       <c r="BJ7">
-        <v>196</v>
+        <v>230</v>
       </c>
       <c r="BK7">
-        <v>170</v>
+        <v>201</v>
       </c>
       <c r="BL7">
-        <v>226</v>
+        <v>263</v>
       </c>
       <c r="BR7">
         <v>269</v>
@@ -8775,34 +8836,49 @@
         <v>99.6</v>
       </c>
       <c r="BT7">
+        <v>196</v>
+      </c>
+      <c r="BU7">
+        <v>170</v>
+      </c>
+      <c r="BV7">
+        <v>226</v>
+      </c>
+      <c r="CB7">
+        <v>269</v>
+      </c>
+      <c r="CC7">
+        <v>99.6</v>
+      </c>
+      <c r="CD7">
         <v>209</v>
       </c>
-      <c r="BU7">
+      <c r="CE7">
         <v>150</v>
       </c>
-      <c r="BV7">
+      <c r="CF7">
         <v>244</v>
       </c>
-      <c r="BW7">
+      <c r="CG7">
         <v>269</v>
       </c>
-      <c r="BX7">
+      <c r="CH7">
         <v>99.6</v>
       </c>
-      <c r="BY7">
+      <c r="CI7">
         <v>175</v>
       </c>
-      <c r="BZ7">
+      <c r="CJ7">
         <v>150</v>
       </c>
-      <c r="CA7">
+      <c r="CK7">
         <v>205</v>
       </c>
-      <c r="CB7" t="s">
+      <c r="CL7" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="8" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:90" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>140</v>
       </c>
@@ -8863,35 +8939,35 @@
       <c r="V8">
         <v>38.9</v>
       </c>
-      <c r="AX8">
-        <v>132</v>
-      </c>
-      <c r="AZ8">
-        <v>4.5</v>
-      </c>
-      <c r="BA8">
-        <v>3.7</v>
-      </c>
-      <c r="BB8">
-        <v>5.5</v>
-      </c>
       <c r="BH8">
         <v>132</v>
       </c>
       <c r="BJ8">
+        <v>4.5</v>
+      </c>
+      <c r="BK8">
+        <v>3.7</v>
+      </c>
+      <c r="BL8">
+        <v>5.5</v>
+      </c>
+      <c r="BR8">
+        <v>132</v>
+      </c>
+      <c r="BT8">
         <v>3.9</v>
       </c>
-      <c r="BK8">
+      <c r="BU8">
         <v>3.2</v>
       </c>
-      <c r="BL8">
+      <c r="BV8">
         <v>4.8</v>
       </c>
-      <c r="CB8" t="s">
+      <c r="CL8" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="9" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:90" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>140</v>
       </c>
@@ -8952,35 +9028,35 @@
       <c r="V9">
         <v>65.099999999999994</v>
       </c>
-      <c r="AX9">
-        <v>372</v>
-      </c>
-      <c r="AZ9">
-        <v>9.6999999999999993</v>
-      </c>
-      <c r="BA9">
-        <v>8.6</v>
-      </c>
-      <c r="BB9">
-        <v>11</v>
-      </c>
       <c r="BH9">
         <v>372</v>
       </c>
       <c r="BJ9">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="BK9">
+        <v>8.6</v>
+      </c>
+      <c r="BL9">
+        <v>11</v>
+      </c>
+      <c r="BR9">
+        <v>372</v>
+      </c>
+      <c r="BT9">
         <v>6.9</v>
       </c>
-      <c r="BK9">
+      <c r="BU9">
         <v>6.2</v>
       </c>
-      <c r="BL9">
+      <c r="BV9">
         <v>7.8</v>
       </c>
-      <c r="CB9" t="s">
+      <c r="CL9" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="10" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:90" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>140</v>
       </c>
@@ -9041,35 +9117,35 @@
       <c r="V10">
         <v>127</v>
       </c>
-      <c r="AX10">
-        <v>236</v>
-      </c>
-      <c r="AZ10">
-        <v>17</v>
-      </c>
-      <c r="BA10">
-        <v>15</v>
-      </c>
-      <c r="BB10">
-        <v>20</v>
-      </c>
       <c r="BH10">
         <v>236</v>
       </c>
       <c r="BJ10">
+        <v>17</v>
+      </c>
+      <c r="BK10">
+        <v>15</v>
+      </c>
+      <c r="BL10">
+        <v>20</v>
+      </c>
+      <c r="BR10">
+        <v>236</v>
+      </c>
+      <c r="BT10">
         <v>11</v>
       </c>
-      <c r="BK10">
+      <c r="BU10">
         <v>9.4</v>
       </c>
-      <c r="BL10">
+      <c r="BV10">
         <v>13</v>
       </c>
-      <c r="CB10" t="s">
+      <c r="CL10" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="11" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:90" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>140</v>
       </c>
@@ -9130,35 +9206,35 @@
       <c r="V11">
         <v>142</v>
       </c>
-      <c r="AX11">
-        <v>269</v>
-      </c>
-      <c r="AZ11">
-        <v>22</v>
-      </c>
-      <c r="BA11">
-        <v>20</v>
-      </c>
-      <c r="BB11">
-        <v>25</v>
-      </c>
       <c r="BH11">
         <v>269</v>
       </c>
       <c r="BJ11">
+        <v>22</v>
+      </c>
+      <c r="BK11">
+        <v>20</v>
+      </c>
+      <c r="BL11">
+        <v>25</v>
+      </c>
+      <c r="BR11">
+        <v>269</v>
+      </c>
+      <c r="BT11">
         <v>18</v>
       </c>
-      <c r="BK11">
-        <v>15</v>
-      </c>
-      <c r="BL11">
+      <c r="BU11">
+        <v>15</v>
+      </c>
+      <c r="BV11">
         <v>20</v>
       </c>
-      <c r="CB11" t="s">
+      <c r="CL11" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="12" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:90" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>210</v>
       </c>
@@ -9279,41 +9355,41 @@
       <c r="AW12">
         <v>0.4</v>
       </c>
-      <c r="BH12">
+      <c r="BR12">
         <v>221</v>
       </c>
-      <c r="BI12">
+      <c r="BS12">
         <v>86.4</v>
       </c>
-      <c r="BJ12">
+      <c r="BT12">
         <v>48</v>
       </c>
-      <c r="BK12">
+      <c r="BU12">
         <v>40</v>
       </c>
-      <c r="BL12">
+      <c r="BV12">
         <v>58</v>
       </c>
-      <c r="BM12">
+      <c r="BW12">
         <v>204</v>
       </c>
-      <c r="BN12">
+      <c r="BX12">
         <v>8.3000000000000007</v>
       </c>
-      <c r="BO12" t="s">
+      <c r="BY12" t="s">
         <v>119</v>
       </c>
-      <c r="BP12" t="s">
+      <c r="BZ12" t="s">
         <v>119</v>
       </c>
-      <c r="BQ12" t="s">
+      <c r="CA12" t="s">
         <v>119</v>
       </c>
-      <c r="CB12" t="s">
+      <c r="CL12" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="13" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:90" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>220</v>
       </c>
@@ -9407,11 +9483,11 @@
       <c r="AS13">
         <v>12.2</v>
       </c>
-      <c r="CB13" t="s">
+      <c r="CL13" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="14" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:90" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>220</v>
       </c>
@@ -9506,7 +9582,7 @@
         <v>12.2</v>
       </c>
     </row>
-    <row r="15" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:90" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>236</v>
       </c>
@@ -9627,38 +9703,38 @@
       <c r="AW15">
         <v>2</v>
       </c>
-      <c r="AX15">
+      <c r="BH15">
         <v>639</v>
       </c>
-      <c r="AY15">
+      <c r="BI15">
         <v>94</v>
       </c>
-      <c r="AZ15">
+      <c r="BJ15">
         <v>22.9</v>
       </c>
-      <c r="BA15">
+      <c r="BK15">
         <v>20.8</v>
       </c>
-      <c r="BB15">
+      <c r="BL15">
         <v>25.1</v>
       </c>
-      <c r="BC15">
+      <c r="BM15">
         <v>358</v>
       </c>
-      <c r="BD15">
+      <c r="BN15">
         <v>11</v>
       </c>
-      <c r="BE15" t="s">
+      <c r="BO15" t="s">
         <v>209</v>
       </c>
-      <c r="BF15" t="s">
+      <c r="BP15" t="s">
         <v>209</v>
       </c>
-      <c r="BG15" t="s">
+      <c r="BQ15" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="16" spans="1:80" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:90" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>236</v>
       </c>
@@ -9779,38 +9855,38 @@
       <c r="AW16">
         <v>2</v>
       </c>
-      <c r="AX16">
+      <c r="BH16">
         <v>639</v>
       </c>
-      <c r="AY16">
+      <c r="BI16">
         <v>99</v>
       </c>
-      <c r="AZ16">
+      <c r="BJ16">
         <v>241</v>
       </c>
-      <c r="BA16">
+      <c r="BK16">
         <v>220</v>
       </c>
-      <c r="BB16">
+      <c r="BL16">
         <v>264</v>
       </c>
-      <c r="BC16">
+      <c r="BM16">
         <v>358</v>
       </c>
-      <c r="BD16">
+      <c r="BN16">
         <v>11</v>
       </c>
-      <c r="BE16" t="s">
+      <c r="BO16" t="s">
         <v>119</v>
       </c>
-      <c r="BF16" t="s">
+      <c r="BP16" t="s">
         <v>119</v>
       </c>
-      <c r="BG16">
+      <c r="BQ16">
         <v>9.4</v>
       </c>
     </row>
-    <row r="17" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>236</v>
       </c>
@@ -9919,38 +9995,38 @@
       <c r="AW17">
         <v>2.2000000000000002</v>
       </c>
-      <c r="AX17">
+      <c r="BH17">
         <v>76</v>
       </c>
-      <c r="AY17">
+      <c r="BI17">
         <v>73.7</v>
       </c>
-      <c r="AZ17">
+      <c r="BJ17">
         <v>7.4</v>
       </c>
-      <c r="BA17" t="s">
+      <c r="BK17" t="s">
         <v>209</v>
       </c>
-      <c r="BB17">
+      <c r="BL17">
         <v>12.5</v>
       </c>
-      <c r="BC17">
+      <c r="BM17">
         <v>57</v>
       </c>
-      <c r="BD17">
+      <c r="BN17">
         <v>3.5</v>
       </c>
-      <c r="BE17" t="s">
+      <c r="BO17" t="s">
         <v>209</v>
       </c>
-      <c r="BF17" t="s">
+      <c r="BP17" t="s">
         <v>209</v>
       </c>
-      <c r="BG17" t="s">
+      <c r="BQ17" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="18" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>236</v>
       </c>
@@ -10056,38 +10132,38 @@
       <c r="AS18" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="AX18">
+      <c r="BH18">
         <v>220</v>
       </c>
-      <c r="AY18">
+      <c r="BI18">
         <v>95</v>
       </c>
-      <c r="AZ18">
+      <c r="BJ18">
         <v>19.899999999999999</v>
       </c>
-      <c r="BA18">
+      <c r="BK18">
         <v>9.3000000000000007</v>
       </c>
-      <c r="BB18">
+      <c r="BL18">
         <v>39.9</v>
       </c>
-      <c r="BC18">
+      <c r="BM18">
         <v>110</v>
       </c>
-      <c r="BD18">
+      <c r="BN18">
         <v>5.5</v>
       </c>
-      <c r="BE18" s="4" t="s">
+      <c r="BO18" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="BF18" s="4" t="s">
+      <c r="BP18" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="BG18" s="4" t="s">
+      <c r="BQ18" s="4" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="19" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>236</v>
       </c>
@@ -10193,38 +10269,38 @@
       <c r="AS19" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="AX19">
+      <c r="BH19">
         <v>343</v>
       </c>
-      <c r="AY19">
+      <c r="BI19">
         <v>98</v>
       </c>
-      <c r="AZ19">
+      <c r="BJ19">
         <v>36.6</v>
       </c>
-      <c r="BA19">
+      <c r="BK19">
         <v>17.600000000000001</v>
       </c>
-      <c r="BB19">
+      <c r="BL19">
         <v>74.599999999999994</v>
       </c>
-      <c r="BC19">
+      <c r="BM19">
         <v>191</v>
       </c>
-      <c r="BD19">
+      <c r="BN19">
         <v>17.3</v>
       </c>
-      <c r="BE19" s="4" t="s">
+      <c r="BO19" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="BF19" s="4" t="s">
+      <c r="BP19" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="BG19" s="4" t="s">
+      <c r="BQ19" s="4" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="20" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>236</v>
       </c>
@@ -10330,38 +10406,38 @@
       <c r="AS20" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="AX20">
+      <c r="BH20">
         <v>76</v>
       </c>
-      <c r="AY20">
+      <c r="BI20">
         <v>98.7</v>
       </c>
-      <c r="AZ20">
+      <c r="BJ20">
         <v>90</v>
       </c>
-      <c r="BA20">
+      <c r="BK20">
         <v>49</v>
       </c>
-      <c r="BB20">
+      <c r="BL20">
         <v>135</v>
       </c>
-      <c r="BC20">
+      <c r="BM20">
         <v>57</v>
       </c>
-      <c r="BD20">
+      <c r="BN20">
         <v>10.5</v>
       </c>
-      <c r="BE20" t="s">
+      <c r="BO20" t="s">
         <v>119</v>
       </c>
-      <c r="BF20" t="s">
+      <c r="BP20" t="s">
         <v>119</v>
       </c>
-      <c r="BG20" t="s">
+      <c r="BQ20" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="21" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>236</v>
       </c>
@@ -10467,38 +10543,38 @@
       <c r="AS21" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="AX21">
+      <c r="BH21">
         <v>220</v>
       </c>
-      <c r="AY21">
+      <c r="BI21">
         <v>98.2</v>
       </c>
-      <c r="AZ21">
+      <c r="BJ21">
         <v>174</v>
       </c>
-      <c r="BA21">
+      <c r="BK21">
         <v>92</v>
       </c>
-      <c r="BB21">
+      <c r="BL21">
         <v>409</v>
       </c>
-      <c r="BC21">
+      <c r="BM21">
         <v>110</v>
       </c>
-      <c r="BD21">
+      <c r="BN21">
         <v>10</v>
       </c>
-      <c r="BE21" t="s">
+      <c r="BO21" t="s">
         <v>119</v>
       </c>
-      <c r="BF21" t="s">
+      <c r="BP21" t="s">
         <v>119</v>
       </c>
-      <c r="BG21" t="s">
+      <c r="BQ21" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="22" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>236</v>
       </c>
@@ -10604,38 +10680,38 @@
       <c r="AS22">
         <v>22.7</v>
       </c>
-      <c r="AX22">
+      <c r="BH22">
         <v>343</v>
       </c>
-      <c r="AY22">
+      <c r="BI22">
         <v>99.7</v>
       </c>
-      <c r="AZ22">
+      <c r="BJ22">
         <v>382</v>
       </c>
-      <c r="BA22">
+      <c r="BK22">
         <v>162</v>
       </c>
-      <c r="BB22">
+      <c r="BL22">
         <v>794</v>
       </c>
-      <c r="BC22">
+      <c r="BM22">
         <v>191</v>
       </c>
-      <c r="BD22">
+      <c r="BN22">
         <v>41.4</v>
       </c>
-      <c r="BE22" t="s">
+      <c r="BO22" t="s">
         <v>119</v>
       </c>
-      <c r="BF22" t="s">
+      <c r="BP22" t="s">
         <v>119</v>
       </c>
-      <c r="BG22">
+      <c r="BQ22">
         <v>21.3</v>
       </c>
     </row>
-    <row r="23" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>249</v>
       </c>
@@ -10702,20 +10778,20 @@
       <c r="AI23">
         <v>99</v>
       </c>
-      <c r="BH23">
+      <c r="BR23">
         <v>56</v>
       </c>
-      <c r="BJ23">
+      <c r="BT23">
         <v>64</v>
       </c>
-      <c r="BK23">
+      <c r="BU23">
         <v>58</v>
       </c>
-      <c r="BL23">
+      <c r="BV23">
         <v>99</v>
       </c>
     </row>
-    <row r="24" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>249</v>
       </c>
@@ -10782,20 +10858,20 @@
       <c r="AI24">
         <v>94.4</v>
       </c>
-      <c r="BH24">
+      <c r="BR24">
         <v>39</v>
       </c>
-      <c r="BJ24">
+      <c r="BT24">
         <v>32</v>
       </c>
-      <c r="BK24">
+      <c r="BU24">
         <v>23</v>
       </c>
-      <c r="BL24">
+      <c r="BV24">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>249</v>
       </c>
@@ -10862,20 +10938,20 @@
       <c r="AI25">
         <v>99.3</v>
       </c>
-      <c r="BH25">
+      <c r="BR25">
         <v>114</v>
       </c>
-      <c r="BJ25">
+      <c r="BT25">
         <v>84</v>
       </c>
-      <c r="BK25">
+      <c r="BU25">
         <v>71</v>
       </c>
-      <c r="BL25">
+      <c r="BV25">
         <v>101</v>
       </c>
     </row>
-    <row r="26" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>249</v>
       </c>
@@ -10942,20 +11018,20 @@
       <c r="AI26">
         <v>95.2</v>
       </c>
-      <c r="BH26">
+      <c r="BR26">
         <v>87</v>
       </c>
-      <c r="BJ26">
+      <c r="BT26">
         <v>48</v>
       </c>
-      <c r="BK26">
+      <c r="BU26">
         <v>39</v>
       </c>
-      <c r="BL26">
+      <c r="BV26">
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>249</v>
       </c>
@@ -11022,20 +11098,20 @@
       <c r="AI27">
         <v>91.9</v>
       </c>
-      <c r="BH27">
+      <c r="BR27">
         <v>73</v>
       </c>
-      <c r="BJ27">
+      <c r="BT27">
         <v>82</v>
       </c>
-      <c r="BK27">
+      <c r="BU27">
         <v>67</v>
       </c>
-      <c r="BL27">
+      <c r="BV27">
         <v>101</v>
       </c>
     </row>
-    <row r="28" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>249</v>
       </c>
@@ -11102,20 +11178,20 @@
       <c r="AI28">
         <v>88.8</v>
       </c>
-      <c r="BH28">
+      <c r="BR28">
         <v>71</v>
       </c>
-      <c r="BJ28">
+      <c r="BT28">
         <v>53</v>
       </c>
-      <c r="BK28">
+      <c r="BU28">
         <v>41</v>
       </c>
-      <c r="BL28">
+      <c r="BV28">
         <v>69</v>
       </c>
     </row>
-    <row r="29" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>249</v>
       </c>
@@ -11182,20 +11258,20 @@
       <c r="AI29">
         <v>97.8</v>
       </c>
-      <c r="BH29">
+      <c r="BR29">
         <v>105</v>
       </c>
-      <c r="BJ29">
+      <c r="BT29">
         <v>45</v>
       </c>
-      <c r="BK29">
+      <c r="BU29">
         <v>37</v>
       </c>
-      <c r="BL29">
+      <c r="BV29">
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>249</v>
       </c>
@@ -11262,20 +11338,20 @@
       <c r="AI30">
         <v>98.2</v>
       </c>
-      <c r="BH30">
+      <c r="BR30">
         <v>115</v>
       </c>
-      <c r="BJ30">
+      <c r="BT30">
         <v>51</v>
       </c>
-      <c r="BK30">
+      <c r="BU30">
         <v>42</v>
       </c>
-      <c r="BL30">
+      <c r="BV30">
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>249</v>
       </c>
@@ -11289,7 +11365,7 @@
         <v>240</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>265</v>
+        <v>13</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>252</v>
@@ -11313,35 +11389,47 @@
         <v>175</v>
       </c>
       <c r="M31">
-        <v>243</v>
+        <v>332</v>
       </c>
       <c r="O31">
-        <v>82</v>
+        <v>10.4</v>
       </c>
       <c r="P31">
-        <v>73</v>
+        <v>9.6</v>
       </c>
       <c r="Q31">
-        <v>92</v>
+        <v>11.3</v>
       </c>
       <c r="AA31">
-        <v>175</v>
+        <v>332</v>
       </c>
       <c r="AC31">
-        <v>1685</v>
+        <v>1293</v>
       </c>
       <c r="AD31">
-        <v>1468</v>
+        <v>1153</v>
       </c>
       <c r="AE31">
-        <v>1797</v>
-      </c>
-    </row>
-    <row r="32" spans="1:64" x14ac:dyDescent="0.2">
+        <v>1449</v>
+      </c>
+      <c r="BH31">
+        <v>212</v>
+      </c>
+      <c r="BJ31">
+        <v>93</v>
+      </c>
+      <c r="BK31">
+        <v>81</v>
+      </c>
+      <c r="BL31">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="32" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="5" t="s">
         <v>250</v>
       </c>
       <c r="C32" t="s">
@@ -11351,7 +11439,7 @@
         <v>222</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>265</v>
+        <v>13</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>252</v>
@@ -11375,31 +11463,43 @@
         <v>175</v>
       </c>
       <c r="M32">
-        <v>197</v>
+        <v>305</v>
       </c>
       <c r="O32">
-        <v>46</v>
+        <v>11.6</v>
       </c>
       <c r="P32">
-        <v>40</v>
+        <v>10.5</v>
       </c>
       <c r="Q32">
-        <v>53</v>
+        <v>12.9</v>
       </c>
       <c r="AA32">
-        <v>57</v>
+        <v>305</v>
       </c>
       <c r="AC32">
-        <v>446</v>
+        <v>411</v>
       </c>
       <c r="AD32">
-        <v>313</v>
+        <v>359</v>
       </c>
       <c r="AE32">
-        <v>615</v>
-      </c>
-    </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.2">
+        <v>471</v>
+      </c>
+      <c r="BH32">
+        <v>194</v>
+      </c>
+      <c r="BJ32">
+        <v>52</v>
+      </c>
+      <c r="BK32">
+        <v>43</v>
+      </c>
+      <c r="BL32">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>249</v>
       </c>
@@ -11413,7 +11513,7 @@
         <v>240</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>265</v>
+        <v>13</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>252</v>
@@ -11437,31 +11537,1021 @@
         <v>175</v>
       </c>
       <c r="M33">
+        <v>307</v>
+      </c>
+      <c r="O33">
+        <v>9.5</v>
+      </c>
+      <c r="P33">
+        <v>9</v>
+      </c>
+      <c r="Q33">
+        <v>10</v>
+      </c>
+      <c r="AA33">
+        <v>307</v>
+      </c>
+      <c r="AC33">
+        <v>1937</v>
+      </c>
+      <c r="AD33">
+        <v>1785</v>
+      </c>
+      <c r="AE33">
+        <v>2103</v>
+      </c>
+      <c r="BH33">
+        <v>122</v>
+      </c>
+      <c r="BJ33">
+        <v>59</v>
+      </c>
+      <c r="BK33">
+        <v>49</v>
+      </c>
+      <c r="BL33">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="1:64" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="C34" t="s">
+        <v>251</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="K34" t="s">
+        <v>15</v>
+      </c>
+      <c r="L34" t="s">
+        <v>175</v>
+      </c>
+      <c r="M34">
+        <v>243</v>
+      </c>
+      <c r="O34">
+        <v>82</v>
+      </c>
+      <c r="P34">
+        <v>73</v>
+      </c>
+      <c r="Q34">
+        <v>92</v>
+      </c>
+      <c r="AA34">
+        <v>175</v>
+      </c>
+      <c r="AC34">
+        <v>1685</v>
+      </c>
+      <c r="AD34">
+        <v>1468</v>
+      </c>
+      <c r="AE34">
+        <v>1797</v>
+      </c>
+    </row>
+    <row r="35" spans="1:64" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="C35" t="s">
+        <v>251</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="K35" t="s">
+        <v>15</v>
+      </c>
+      <c r="L35" t="s">
+        <v>175</v>
+      </c>
+      <c r="M35">
+        <v>197</v>
+      </c>
+      <c r="O35">
+        <v>46</v>
+      </c>
+      <c r="P35">
+        <v>40</v>
+      </c>
+      <c r="Q35">
+        <v>53</v>
+      </c>
+      <c r="AA35">
+        <v>57</v>
+      </c>
+      <c r="AC35">
+        <v>446</v>
+      </c>
+      <c r="AD35">
+        <v>313</v>
+      </c>
+      <c r="AE35">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="36" spans="1:64" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="C36" t="s">
+        <v>251</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="K36" t="s">
+        <v>15</v>
+      </c>
+      <c r="L36" t="s">
+        <v>175</v>
+      </c>
+      <c r="M36">
         <v>220</v>
       </c>
-      <c r="O33">
+      <c r="O36">
         <v>49</v>
       </c>
-      <c r="P33">
+      <c r="P36">
         <v>43</v>
       </c>
-      <c r="Q33">
+      <c r="Q36">
         <v>56</v>
       </c>
-      <c r="AA33">
+      <c r="AA36">
         <v>187</v>
       </c>
-      <c r="AC33">
+      <c r="AC36">
         <v>1722</v>
       </c>
-      <c r="AD33">
+      <c r="AD36">
         <v>1503</v>
       </c>
-      <c r="AE33">
+      <c r="AE36">
         <v>1972</v>
       </c>
     </row>
+    <row r="37" spans="1:64" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B37" t="s">
+        <v>312</v>
+      </c>
+      <c r="C37">
+        <v>1999</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="G37">
+        <v>18</v>
+      </c>
+      <c r="H37">
+        <v>35</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="K37" t="s">
+        <v>313</v>
+      </c>
+      <c r="L37" t="s">
+        <v>171</v>
+      </c>
+      <c r="M37">
+        <v>22</v>
+      </c>
+      <c r="O37">
+        <v>9.6</v>
+      </c>
+      <c r="P37">
+        <v>5</v>
+      </c>
+      <c r="Q37">
+        <v>21</v>
+      </c>
+      <c r="AA37">
+        <v>22</v>
+      </c>
+      <c r="AC37">
+        <v>465</v>
+      </c>
+      <c r="AD37">
+        <v>293</v>
+      </c>
+      <c r="AE37">
+        <v>894</v>
+      </c>
+      <c r="BC37">
+        <v>22</v>
+      </c>
+      <c r="BE37">
+        <v>119</v>
+      </c>
+      <c r="BF37">
+        <v>53</v>
+      </c>
+      <c r="BG37">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="38" spans="1:64" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B38" t="s">
+        <v>312</v>
+      </c>
+      <c r="C38">
+        <v>1999</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="G38">
+        <v>18</v>
+      </c>
+      <c r="H38">
+        <v>35</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="K38" t="s">
+        <v>314</v>
+      </c>
+      <c r="L38" t="s">
+        <v>171</v>
+      </c>
+      <c r="M38">
+        <v>22</v>
+      </c>
+      <c r="O38">
+        <v>0.2</v>
+      </c>
+      <c r="P38">
+        <v>0.1</v>
+      </c>
+      <c r="Q38">
+        <v>0.3</v>
+      </c>
+      <c r="AA38">
+        <v>22</v>
+      </c>
+      <c r="AC38">
+        <v>8.9</v>
+      </c>
+      <c r="AD38">
+        <v>1.9</v>
+      </c>
+      <c r="AE38">
+        <v>18</v>
+      </c>
+      <c r="BC38">
+        <v>22</v>
+      </c>
+      <c r="BE38">
+        <v>5</v>
+      </c>
+      <c r="BF38">
+        <v>1.2</v>
+      </c>
+      <c r="BG38">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:64" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B39" t="s">
+        <v>312</v>
+      </c>
+      <c r="C39">
+        <v>1999</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="G39">
+        <v>5</v>
+      </c>
+      <c r="H39">
+        <v>14</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="K39" t="s">
+        <v>313</v>
+      </c>
+      <c r="L39" t="s">
+        <v>171</v>
+      </c>
+      <c r="M39">
+        <v>55</v>
+      </c>
+      <c r="O39">
+        <v>0.7</v>
+      </c>
+      <c r="P39">
+        <v>0.2</v>
+      </c>
+      <c r="Q39">
+        <v>1.8</v>
+      </c>
+      <c r="AA39">
+        <v>55</v>
+      </c>
+      <c r="AC39">
+        <v>169</v>
+      </c>
+      <c r="AD39">
+        <v>81</v>
+      </c>
+      <c r="AE39">
+        <v>290</v>
+      </c>
+      <c r="BC39">
+        <v>55</v>
+      </c>
+      <c r="BE39">
+        <v>30</v>
+      </c>
+      <c r="BF39">
+        <v>14</v>
+      </c>
+      <c r="BG39">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="40" spans="1:64" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B40" t="s">
+        <v>312</v>
+      </c>
+      <c r="C40">
+        <v>1999</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="G40">
+        <v>5</v>
+      </c>
+      <c r="H40">
+        <v>14</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="K40" t="s">
+        <v>314</v>
+      </c>
+      <c r="L40" t="s">
+        <v>171</v>
+      </c>
+      <c r="M40">
+        <v>55</v>
+      </c>
+      <c r="O40">
+        <v>0.05</v>
+      </c>
+      <c r="P40">
+        <v>0.02</v>
+      </c>
+      <c r="Q40">
+        <v>0.1</v>
+      </c>
+      <c r="AA40">
+        <v>55</v>
+      </c>
+      <c r="AC40">
+        <v>17</v>
+      </c>
+      <c r="AD40">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="AE40">
+        <v>44</v>
+      </c>
+      <c r="BC40">
+        <v>55</v>
+      </c>
+      <c r="BE40">
+        <v>5</v>
+      </c>
+      <c r="BF40">
+        <v>3.3</v>
+      </c>
+      <c r="BG40">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="1:64" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B41" t="s">
+        <v>312</v>
+      </c>
+      <c r="C41">
+        <v>1999</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="G41">
+        <v>5</v>
+      </c>
+      <c r="H41">
+        <v>14</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="K41" t="s">
+        <v>313</v>
+      </c>
+      <c r="L41" t="s">
+        <v>171</v>
+      </c>
+      <c r="M41">
+        <v>50</v>
+      </c>
+      <c r="O41">
+        <v>0.44</v>
+      </c>
+      <c r="P41">
+        <v>0.3</v>
+      </c>
+      <c r="Q41">
+        <v>0.6</v>
+      </c>
+      <c r="AA41">
+        <v>50</v>
+      </c>
+      <c r="AC41">
+        <v>19</v>
+      </c>
+      <c r="AD41">
+        <v>7.8</v>
+      </c>
+      <c r="AE41">
+        <v>44</v>
+      </c>
+      <c r="BC41">
+        <v>50</v>
+      </c>
+      <c r="BE41">
+        <v>13</v>
+      </c>
+      <c r="BF41">
+        <v>6</v>
+      </c>
+      <c r="BG41">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="42" spans="1:64" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B42" t="s">
+        <v>312</v>
+      </c>
+      <c r="C42">
+        <v>1999</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="G42">
+        <v>5</v>
+      </c>
+      <c r="H42">
+        <v>14</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="K42" t="s">
+        <v>314</v>
+      </c>
+      <c r="L42" t="s">
+        <v>171</v>
+      </c>
+      <c r="M42">
+        <v>50</v>
+      </c>
+      <c r="O42">
+        <v>0.05</v>
+      </c>
+      <c r="P42">
+        <v>0.03</v>
+      </c>
+      <c r="Q42">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AA42">
+        <v>50</v>
+      </c>
+      <c r="AC42">
+        <v>2.6</v>
+      </c>
+      <c r="AD42">
+        <v>0.8</v>
+      </c>
+      <c r="AE42">
+        <v>7.6</v>
+      </c>
+      <c r="BC42">
+        <v>50</v>
+      </c>
+      <c r="BE42">
+        <v>2</v>
+      </c>
+      <c r="BF42">
+        <v>0.8</v>
+      </c>
+      <c r="BG42">
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:64" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B43" t="s">
+        <v>312</v>
+      </c>
+      <c r="C43">
+        <v>1999</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="G43">
+        <v>2</v>
+      </c>
+      <c r="H43">
+        <v>4</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="K43" t="s">
+        <v>313</v>
+      </c>
+      <c r="L43" t="s">
+        <v>171</v>
+      </c>
+      <c r="M43">
+        <v>48</v>
+      </c>
+      <c r="O43">
+        <v>0.2</v>
+      </c>
+      <c r="P43">
+        <v>0.1</v>
+      </c>
+      <c r="Q43">
+        <v>0.3</v>
+      </c>
+      <c r="AA43">
+        <v>48</v>
+      </c>
+      <c r="AC43">
+        <v>77</v>
+      </c>
+      <c r="AD43">
+        <v>41</v>
+      </c>
+      <c r="AE43">
+        <v>165</v>
+      </c>
+      <c r="AX43">
+        <v>48</v>
+      </c>
+      <c r="AZ43">
+        <v>54</v>
+      </c>
+      <c r="BA43">
+        <v>35</v>
+      </c>
+      <c r="BB43">
+        <v>165</v>
+      </c>
+      <c r="BC43">
+        <v>48</v>
+      </c>
+      <c r="BE43">
+        <v>20</v>
+      </c>
+      <c r="BF43">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="BG43">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="1:64" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B44" t="s">
+        <v>312</v>
+      </c>
+      <c r="C44">
+        <v>1999</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="G44">
+        <v>2</v>
+      </c>
+      <c r="H44">
+        <v>4</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="K44" t="s">
+        <v>314</v>
+      </c>
+      <c r="L44" t="s">
+        <v>171</v>
+      </c>
+      <c r="M44">
+        <v>48</v>
+      </c>
+      <c r="O44">
+        <v>0.02</v>
+      </c>
+      <c r="P44">
+        <v>0.01</v>
+      </c>
+      <c r="Q44">
+        <v>0.02</v>
+      </c>
+      <c r="AA44">
+        <v>48</v>
+      </c>
+      <c r="AC44">
+        <v>6.2</v>
+      </c>
+      <c r="AD44">
+        <v>2.8</v>
+      </c>
+      <c r="AE44">
+        <v>18</v>
+      </c>
+      <c r="AX44">
+        <v>48</v>
+      </c>
+      <c r="AZ44">
+        <v>4.2</v>
+      </c>
+      <c r="BA44">
+        <v>1.9</v>
+      </c>
+      <c r="BB44">
+        <v>9.9</v>
+      </c>
+      <c r="BC44">
+        <v>48</v>
+      </c>
+      <c r="BE44">
+        <v>3</v>
+      </c>
+      <c r="BF44">
+        <v>1.4</v>
+      </c>
+      <c r="BG44">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:64" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B45" t="s">
+        <v>312</v>
+      </c>
+      <c r="C45">
+        <v>1999</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="G45">
+        <v>2</v>
+      </c>
+      <c r="H45">
+        <v>4</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="K45" t="s">
+        <v>313</v>
+      </c>
+      <c r="L45" t="s">
+        <v>171</v>
+      </c>
+      <c r="M45">
+        <v>52</v>
+      </c>
+      <c r="O45">
+        <v>0.2</v>
+      </c>
+      <c r="P45">
+        <v>0.1</v>
+      </c>
+      <c r="Q45">
+        <v>0.2</v>
+      </c>
+      <c r="AA45">
+        <v>52</v>
+      </c>
+      <c r="AC45">
+        <v>70</v>
+      </c>
+      <c r="AD45">
+        <v>37</v>
+      </c>
+      <c r="AE45">
+        <v>126</v>
+      </c>
+      <c r="AX45">
+        <v>52</v>
+      </c>
+      <c r="AZ45">
+        <v>95</v>
+      </c>
+      <c r="BA45">
+        <v>60</v>
+      </c>
+      <c r="BB45">
+        <v>126</v>
+      </c>
+      <c r="BC45">
+        <v>52</v>
+      </c>
+      <c r="BE45">
+        <v>31</v>
+      </c>
+      <c r="BF45">
+        <v>22</v>
+      </c>
+      <c r="BG45">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="46" spans="1:64" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B46" t="s">
+        <v>312</v>
+      </c>
+      <c r="C46">
+        <v>1999</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="G46">
+        <v>2</v>
+      </c>
+      <c r="H46">
+        <v>4</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="K46" t="s">
+        <v>314</v>
+      </c>
+      <c r="L46" t="s">
+        <v>171</v>
+      </c>
+      <c r="M46">
+        <v>52</v>
+      </c>
+      <c r="O46">
+        <v>0.02</v>
+      </c>
+      <c r="P46">
+        <v>0.01</v>
+      </c>
+      <c r="Q46">
+        <v>0.02</v>
+      </c>
+      <c r="AA46">
+        <v>52</v>
+      </c>
+      <c r="AC46">
+        <v>5.7</v>
+      </c>
+      <c r="AD46">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AE46">
+        <v>13</v>
+      </c>
+      <c r="AX46">
+        <v>52</v>
+      </c>
+      <c r="AZ46">
+        <v>5</v>
+      </c>
+      <c r="BA46">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="BB46">
+        <v>12</v>
+      </c>
+      <c r="BC46">
+        <v>52</v>
+      </c>
+      <c r="BE46">
+        <v>2.6</v>
+      </c>
+      <c r="BF46">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="BG46">
+        <v>7.3</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B35" r:id="rId1" xr:uid="{8F314CA9-A3F4-ED42-B525-6DD22C990BB0}"/>
+    <hyperlink ref="B32" r:id="rId2" xr:uid="{C3AFD843-E8BC-D748-867C-4238E1D9D42A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
commiting chaos of night before presentation. HERE BE DRAGONS!
</commit_message>
<xml_diff>
--- a/data/typhoid_vaccine_study_data.xlsx
+++ b/data/typhoid_vaccine_study_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/famulare/git/famulare/typhoid-immune-dynamics/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{277BC6EA-B8DA-DF42-9C1B-37C1EBA13DF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE7AA06-FDA7-0A41-B411-270E80FA35EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20060" yWindow="840" windowWidth="14500" windowHeight="17440" activeTab="2" xr2:uid="{3C28E045-1CB7-C04C-9830-A174AB0F25A4}"/>
+    <workbookView xWindow="15000" yWindow="840" windowWidth="19560" windowHeight="17440" xr2:uid="{3C28E045-1CB7-C04C-9830-A174AB0F25A4}"/>
   </bookViews>
   <sheets>
     <sheet name="efficacy" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3935" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3928" uniqueCount="332">
   <si>
     <t>study</t>
   </si>
@@ -1098,7 +1098,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1109,6 +1109,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1446,9 +1447,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E976F573-8D26-E847-8FB6-13AA5974A482}">
   <dimension ref="A1:AH68"/>
   <sheetViews>
-    <sheetView topLeftCell="A50" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F66" sqref="F66"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="J60" sqref="J60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6179,8 +6180,8 @@
       <c r="I53" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="J53" s="1" t="s">
-        <v>65</v>
+      <c r="J53" s="10">
+        <v>12</v>
       </c>
       <c r="K53" s="1" t="s">
         <v>11</v>
@@ -6387,8 +6388,8 @@
       <c r="I55" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="J55" s="1" t="s">
-        <v>65</v>
+      <c r="J55" s="10">
+        <v>12</v>
       </c>
       <c r="K55" s="1" t="s">
         <v>11</v>
@@ -6491,8 +6492,8 @@
       <c r="I56" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="J56" s="1" t="s">
-        <v>65</v>
+      <c r="J56" s="10">
+        <v>12</v>
       </c>
       <c r="K56" s="1" t="s">
         <v>11</v>
@@ -6595,8 +6596,8 @@
       <c r="I57" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="J57" s="1" t="s">
-        <v>65</v>
+      <c r="J57" s="10">
+        <v>12</v>
       </c>
       <c r="K57" s="1" t="s">
         <v>11</v>
@@ -6699,8 +6700,8 @@
       <c r="I58" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="J58" s="1" t="s">
-        <v>65</v>
+      <c r="J58" s="10">
+        <v>12</v>
       </c>
       <c r="K58" s="1" t="s">
         <v>11</v>
@@ -6803,8 +6804,8 @@
       <c r="I59" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="J59" s="1" t="s">
-        <v>65</v>
+      <c r="J59" s="10">
+        <v>12</v>
       </c>
       <c r="K59" s="1" t="s">
         <v>11</v>
@@ -6907,8 +6908,8 @@
       <c r="I60" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="J60" s="1" t="s">
-        <v>65</v>
+      <c r="J60" s="10">
+        <v>12</v>
       </c>
       <c r="K60" s="1" t="s">
         <v>11</v>
@@ -7821,10 +7822,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{149A3A41-8A6C-584E-BBE8-03656533BC7D}">
   <dimension ref="A1:CL46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="S1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="BJ6" sqref="BJ6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12579,8 +12580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22F67001-9217-094F-9712-0E917E529FDB}">
   <dimension ref="A1:XFC900"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A857" workbookViewId="0">
-      <selection activeCell="B399" sqref="B399"/>
+    <sheetView topLeftCell="A422" workbookViewId="0">
+      <selection activeCell="F578" sqref="F578"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>